<commit_message>
Added Diary entry for Lecture2_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -115,25 +115,67 @@
     <t>Feeling tired! Should not underestimate the work. A lot to learn and willing to learn!</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
+    <t>1/16/2020</t>
+  </si>
+  <si>
+    <t>Looking forward to listen to Ping Chen’s talk! Couldn’t guess what the content would be on, but I believe it would be more in depth discussion towards reading code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learnt various comprehension styles with the help of simple examples like Billing systems for Fridge, Gaming, Squirrel.             Explored different versions of Pacman and answered the questions in the lecture. Learnt common gaming classes used. Finally, got to hear from Ping Chen about his journey, code reading, tech debt, etc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understood tons of files present doesn’t imply we need to understand each and every single line. With practice, one can learn how to effectively surf through the relevant information. Hearing from Ping Chen that this is close enough to reality sounds assuring that this is an essential skill that has to be mastered. </t>
+  </si>
+  <si>
+    <t>Informative, Looking forward to hear more from Alumni!</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Shikun, Yitian</t>
+  </si>
+  <si>
+    <t>To decide the project</t>
+  </si>
+  <si>
+    <t>Decided to settle with an android app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We were facing a number of problems while selecting the projects, some would match the requirements but wouldn’t run on the system or would be harder to understand. </t>
+  </si>
+  <si>
+    <t>Settled with a project, feels overwhelming, hopefully able to achieve the project goals with the selected topic.</t>
+  </si>
+  <si>
+    <t>15:00 - 16:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To read the articles given </t>
+  </si>
+  <si>
+    <t>Finished reading the three articles. Learnt about Singleton patterns</t>
+  </si>
+  <si>
+    <t>The Github article was rather tedious to read, the other two were interesting but indeed provided lot of meaningful insights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nice read! Tired </t>
+  </si>
+  <si>
+    <t>21:00 - 23:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To finish Pacman homework </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understood the Pacman game and the various classes. Used the techniques given in class to efficiently finish the homework. </t>
+  </si>
+  <si>
+    <t>The last question about fruit implementation required a bit of thinking compared to the other as there were many possible implementations. Sufficient homework style to test what we learnt in class!</t>
+  </si>
+  <si>
+    <t>Feeling good! Think the answers were right.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +487,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -515,14 +557,29 @@
     <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -530,14 +587,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -774,17 +828,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -812,10 +866,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1063,12 +1117,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1355,7 +1409,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1383,10 +1437,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1825,1036 +1879,1078 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" ht="15.5" customHeight="1">
+    <row r="13" ht="129" customHeight="1">
       <c r="A13" t="s" s="23">
         <v>31</v>
       </c>
-      <c r="B13" t="s" s="24">
+      <c r="B13" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="C13" t="s" s="24">
+      <c r="E13" t="s" s="21">
         <v>33</v>
       </c>
-      <c r="D13" t="s" s="24">
+      <c r="F13" t="s" s="21">
         <v>34</v>
       </c>
-      <c r="E13" t="s" s="24">
+      <c r="G13" t="s" s="24">
         <v>35</v>
       </c>
-      <c r="F13" t="s" s="24">
+    </row>
+    <row r="14" ht="73" customHeight="1">
+      <c r="A14" s="19">
+        <v>43847</v>
+      </c>
+      <c r="B14" t="s" s="20">
         <v>36</v>
       </c>
-      <c r="G13" t="s" s="25">
+      <c r="C14" t="s" s="20">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" ht="15.5" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-    </row>
-    <row r="15" ht="15.5" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" ht="15.5" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="D14" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s" s="25">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s" s="25">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s" s="26">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" ht="71.75" customHeight="1">
+      <c r="A15" s="19">
+        <v>43849</v>
+      </c>
+      <c r="B15" t="s" s="20">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s" s="25">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s" s="25">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s" s="25">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s" s="26">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" ht="93.05" customHeight="1">
+      <c r="A16" s="19">
+        <v>43851</v>
+      </c>
+      <c r="B16" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s" s="25">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s" s="25">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s" s="25">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s" s="26">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" ht="15.5" customHeight="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" ht="15.5" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" ht="15.5" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" ht="15.5" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" ht="15.5" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="34"/>
     </row>
     <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="34"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="34"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="34"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="34"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="26"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="28"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="34"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="28"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="34"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="34"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="26"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="28"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="34"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="28"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="34"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="28"/>
+      <c r="A45" s="31"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="34"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="26"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="28"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="34"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="34"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="26"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="34"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="28"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="34"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="34"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="28"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="34"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="28"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="28"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="34"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="28"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="34"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="26"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="28"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="34"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="28"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="34"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="26"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="28"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="34"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="28"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="34"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="26"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="28"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="34"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="26"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="28"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="34"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="26"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="28"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="34"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="26"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="28"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="34"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="26"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="28"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="34"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="26"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="28"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="34"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="26"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="28"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="34"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="26"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="28"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="34"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="28"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="34"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="26"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="28"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="34"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="26"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="28"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="26"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="28"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="26"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="28"/>
+      <c r="A71" s="31"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="34"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="26"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="28"/>
+      <c r="A72" s="31"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="34"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="26"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="28"/>
+      <c r="A73" s="31"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+      <c r="G73" s="34"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="26"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="28"/>
+      <c r="A74" s="31"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="34"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="26"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="28"/>
+      <c r="A75" s="31"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="34"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="26"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="28"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="34"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="26"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="28"/>
+      <c r="A77" s="31"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="34"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="26"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="28"/>
+      <c r="A78" s="31"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="34"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="26"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="28"/>
+      <c r="A79" s="31"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="34"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="26"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="28"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32"/>
+      <c r="G80" s="34"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="26"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="28"/>
+      <c r="A81" s="31"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="32"/>
+      <c r="G81" s="34"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="26"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="28"/>
+      <c r="A82" s="31"/>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="32"/>
+      <c r="G82" s="34"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="26"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="28"/>
+      <c r="A83" s="31"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="32"/>
+      <c r="G83" s="34"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="26"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="28"/>
+      <c r="A84" s="31"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="34"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="26"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="28"/>
+      <c r="A85" s="31"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="32"/>
+      <c r="G85" s="34"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="26"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="28"/>
+      <c r="A86" s="31"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="32"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="32"/>
+      <c r="G86" s="34"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="26"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="28"/>
+      <c r="A87" s="31"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="32"/>
+      <c r="G87" s="34"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="26"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="28"/>
+      <c r="A88" s="31"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
+      <c r="G88" s="34"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="26"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="28"/>
+      <c r="A89" s="31"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="32"/>
+      <c r="G89" s="34"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="26"/>
-      <c r="B90" s="27"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="28"/>
+      <c r="A90" s="31"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32"/>
+      <c r="G90" s="34"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="26"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="28"/>
+      <c r="A91" s="31"/>
+      <c r="B91" s="32"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="34"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="26"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="28"/>
+      <c r="A92" s="31"/>
+      <c r="B92" s="32"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="32"/>
+      <c r="F92" s="32"/>
+      <c r="G92" s="34"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="26"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="28"/>
+      <c r="A93" s="31"/>
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="34"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="26"/>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="28"/>
+      <c r="A94" s="31"/>
+      <c r="B94" s="32"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="32"/>
+      <c r="G94" s="34"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="26"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="28"/>
+      <c r="A95" s="31"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="34"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="26"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="28"/>
+      <c r="A96" s="31"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="34"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="26"/>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="28"/>
+      <c r="A97" s="31"/>
+      <c r="B97" s="32"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="34"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="26"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="28"/>
+      <c r="A98" s="31"/>
+      <c r="B98" s="32"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="34"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="26"/>
-      <c r="B99" s="27"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="28"/>
+      <c r="A99" s="31"/>
+      <c r="B99" s="32"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="32"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="32"/>
+      <c r="G99" s="34"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="26"/>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="28"/>
+      <c r="A100" s="31"/>
+      <c r="B100" s="32"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="32"/>
+      <c r="E100" s="32"/>
+      <c r="F100" s="32"/>
+      <c r="G100" s="34"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="26"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="28"/>
+      <c r="A101" s="31"/>
+      <c r="B101" s="32"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="32"/>
+      <c r="G101" s="34"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="26"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="28"/>
+      <c r="A102" s="31"/>
+      <c r="B102" s="32"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="32"/>
+      <c r="G102" s="34"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="26"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="28"/>
+      <c r="A103" s="31"/>
+      <c r="B103" s="32"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="32"/>
+      <c r="G103" s="34"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="26"/>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="28"/>
+      <c r="A104" s="31"/>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="34"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="26"/>
-      <c r="B105" s="27"/>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="28"/>
+      <c r="A105" s="31"/>
+      <c r="B105" s="32"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="32"/>
+      <c r="G105" s="34"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="26"/>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="28"/>
+      <c r="A106" s="31"/>
+      <c r="B106" s="32"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="32"/>
+      <c r="G106" s="34"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="26"/>
-      <c r="B107" s="27"/>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="28"/>
+      <c r="A107" s="31"/>
+      <c r="B107" s="32"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="32"/>
+      <c r="G107" s="34"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="26"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="28"/>
+      <c r="A108" s="31"/>
+      <c r="B108" s="32"/>
+      <c r="C108" s="32"/>
+      <c r="D108" s="32"/>
+      <c r="E108" s="32"/>
+      <c r="F108" s="32"/>
+      <c r="G108" s="34"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="26"/>
-      <c r="B109" s="27"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="28"/>
+      <c r="A109" s="31"/>
+      <c r="B109" s="32"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="32"/>
+      <c r="E109" s="32"/>
+      <c r="F109" s="32"/>
+      <c r="G109" s="34"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="26"/>
-      <c r="B110" s="27"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-      <c r="F110" s="27"/>
-      <c r="G110" s="28"/>
+      <c r="A110" s="31"/>
+      <c r="B110" s="32"/>
+      <c r="C110" s="32"/>
+      <c r="D110" s="32"/>
+      <c r="E110" s="32"/>
+      <c r="F110" s="32"/>
+      <c r="G110" s="34"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="26"/>
-      <c r="B111" s="27"/>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="28"/>
+      <c r="A111" s="31"/>
+      <c r="B111" s="32"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="32"/>
+      <c r="E111" s="32"/>
+      <c r="F111" s="32"/>
+      <c r="G111" s="34"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="26"/>
-      <c r="B112" s="27"/>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="28"/>
+      <c r="A112" s="31"/>
+      <c r="B112" s="32"/>
+      <c r="C112" s="32"/>
+      <c r="D112" s="32"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="32"/>
+      <c r="G112" s="34"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="26"/>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="28"/>
+      <c r="A113" s="31"/>
+      <c r="B113" s="32"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="32"/>
+      <c r="E113" s="32"/>
+      <c r="F113" s="32"/>
+      <c r="G113" s="34"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="26"/>
-      <c r="B114" s="27"/>
-      <c r="C114" s="27"/>
-      <c r="D114" s="27"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
-      <c r="G114" s="28"/>
+      <c r="A114" s="31"/>
+      <c r="B114" s="32"/>
+      <c r="C114" s="32"/>
+      <c r="D114" s="32"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="32"/>
+      <c r="G114" s="34"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="26"/>
-      <c r="B115" s="27"/>
-      <c r="C115" s="27"/>
-      <c r="D115" s="27"/>
-      <c r="E115" s="27"/>
-      <c r="F115" s="27"/>
-      <c r="G115" s="28"/>
+      <c r="A115" s="31"/>
+      <c r="B115" s="32"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="32"/>
+      <c r="E115" s="32"/>
+      <c r="F115" s="32"/>
+      <c r="G115" s="34"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="26"/>
-      <c r="B116" s="27"/>
-      <c r="C116" s="27"/>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-      <c r="F116" s="27"/>
-      <c r="G116" s="28"/>
+      <c r="A116" s="31"/>
+      <c r="B116" s="32"/>
+      <c r="C116" s="32"/>
+      <c r="D116" s="32"/>
+      <c r="E116" s="32"/>
+      <c r="F116" s="32"/>
+      <c r="G116" s="34"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="26"/>
-      <c r="B117" s="27"/>
-      <c r="C117" s="27"/>
-      <c r="D117" s="27"/>
-      <c r="E117" s="27"/>
-      <c r="F117" s="27"/>
-      <c r="G117" s="28"/>
+      <c r="A117" s="31"/>
+      <c r="B117" s="32"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="32"/>
+      <c r="E117" s="32"/>
+      <c r="F117" s="32"/>
+      <c r="G117" s="34"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="26"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="27"/>
-      <c r="E118" s="27"/>
-      <c r="F118" s="27"/>
-      <c r="G118" s="28"/>
+      <c r="A118" s="31"/>
+      <c r="B118" s="32"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="32"/>
+      <c r="E118" s="32"/>
+      <c r="F118" s="32"/>
+      <c r="G118" s="34"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="26"/>
-      <c r="B119" s="27"/>
-      <c r="C119" s="27"/>
-      <c r="D119" s="27"/>
-      <c r="E119" s="27"/>
-      <c r="F119" s="27"/>
-      <c r="G119" s="28"/>
+      <c r="A119" s="31"/>
+      <c r="B119" s="32"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="32"/>
+      <c r="E119" s="32"/>
+      <c r="F119" s="32"/>
+      <c r="G119" s="34"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="26"/>
-      <c r="B120" s="27"/>
-      <c r="C120" s="27"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="28"/>
+      <c r="A120" s="31"/>
+      <c r="B120" s="32"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="32"/>
+      <c r="E120" s="32"/>
+      <c r="F120" s="32"/>
+      <c r="G120" s="34"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="26"/>
-      <c r="B121" s="27"/>
-      <c r="C121" s="27"/>
-      <c r="D121" s="27"/>
-      <c r="E121" s="27"/>
-      <c r="F121" s="27"/>
-      <c r="G121" s="28"/>
+      <c r="A121" s="31"/>
+      <c r="B121" s="32"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="32"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="32"/>
+      <c r="G121" s="34"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="26"/>
-      <c r="B122" s="27"/>
-      <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="27"/>
-      <c r="G122" s="28"/>
+      <c r="A122" s="31"/>
+      <c r="B122" s="32"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="32"/>
+      <c r="E122" s="32"/>
+      <c r="F122" s="32"/>
+      <c r="G122" s="34"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="26"/>
-      <c r="B123" s="27"/>
-      <c r="C123" s="27"/>
-      <c r="D123" s="27"/>
-      <c r="E123" s="27"/>
-      <c r="F123" s="27"/>
-      <c r="G123" s="28"/>
+      <c r="A123" s="31"/>
+      <c r="B123" s="32"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="32"/>
+      <c r="E123" s="32"/>
+      <c r="F123" s="32"/>
+      <c r="G123" s="34"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="26"/>
-      <c r="B124" s="27"/>
-      <c r="C124" s="27"/>
-      <c r="D124" s="27"/>
-      <c r="E124" s="27"/>
-      <c r="F124" s="27"/>
-      <c r="G124" s="28"/>
+      <c r="A124" s="31"/>
+      <c r="B124" s="32"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="32"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="32"/>
+      <c r="G124" s="34"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="32"/>
-      <c r="B125" s="33"/>
-      <c r="C125" s="33"/>
-      <c r="D125" s="33"/>
-      <c r="E125" s="33"/>
-      <c r="F125" s="33"/>
-      <c r="G125" s="34"/>
+      <c r="A125" s="36"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="37"/>
+      <c r="D125" s="37"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="37"/>
+      <c r="G125" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Diary entry for Lecture2_Santhiya_Nagarajan (#156)
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -115,25 +115,67 @@
     <t>Feeling tired! Should not underestimate the work. A lot to learn and willing to learn!</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
+    <t>1/16/2020</t>
+  </si>
+  <si>
+    <t>Looking forward to listen to Ping Chen’s talk! Couldn’t guess what the content would be on, but I believe it would be more in depth discussion towards reading code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learnt various comprehension styles with the help of simple examples like Billing systems for Fridge, Gaming, Squirrel.             Explored different versions of Pacman and answered the questions in the lecture. Learnt common gaming classes used. Finally, got to hear from Ping Chen about his journey, code reading, tech debt, etc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understood tons of files present doesn’t imply we need to understand each and every single line. With practice, one can learn how to effectively surf through the relevant information. Hearing from Ping Chen that this is close enough to reality sounds assuring that this is an essential skill that has to be mastered. </t>
+  </si>
+  <si>
+    <t>Informative, Looking forward to hear more from Alumni!</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Shikun, Yitian</t>
+  </si>
+  <si>
+    <t>To decide the project</t>
+  </si>
+  <si>
+    <t>Decided to settle with an android app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We were facing a number of problems while selecting the projects, some would match the requirements but wouldn’t run on the system or would be harder to understand. </t>
+  </si>
+  <si>
+    <t>Settled with a project, feels overwhelming, hopefully able to achieve the project goals with the selected topic.</t>
+  </si>
+  <si>
+    <t>15:00 - 16:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To read the articles given </t>
+  </si>
+  <si>
+    <t>Finished reading the three articles. Learnt about Singleton patterns</t>
+  </si>
+  <si>
+    <t>The Github article was rather tedious to read, the other two were interesting but indeed provided lot of meaningful insights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nice read! Tired </t>
+  </si>
+  <si>
+    <t>21:00 - 23:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To finish Pacman homework </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understood the Pacman game and the various classes. Used the techniques given in class to efficiently finish the homework. </t>
+  </si>
+  <si>
+    <t>The last question about fruit implementation required a bit of thinking compared to the other as there were many possible implementations. Sufficient homework style to test what we learnt in class!</t>
+  </si>
+  <si>
+    <t>Feeling good! Think the answers were right.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +487,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -515,14 +557,29 @@
     <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -530,14 +587,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -774,17 +828,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -812,10 +866,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1063,12 +1117,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1355,7 +1409,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1383,10 +1437,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1825,1036 +1879,1078 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" ht="15.5" customHeight="1">
+    <row r="13" ht="129" customHeight="1">
       <c r="A13" t="s" s="23">
         <v>31</v>
       </c>
-      <c r="B13" t="s" s="24">
+      <c r="B13" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="C13" t="s" s="24">
+      <c r="E13" t="s" s="21">
         <v>33</v>
       </c>
-      <c r="D13" t="s" s="24">
+      <c r="F13" t="s" s="21">
         <v>34</v>
       </c>
-      <c r="E13" t="s" s="24">
+      <c r="G13" t="s" s="24">
         <v>35</v>
       </c>
-      <c r="F13" t="s" s="24">
+    </row>
+    <row r="14" ht="73" customHeight="1">
+      <c r="A14" s="19">
+        <v>43847</v>
+      </c>
+      <c r="B14" t="s" s="20">
         <v>36</v>
       </c>
-      <c r="G13" t="s" s="25">
+      <c r="C14" t="s" s="20">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" ht="15.5" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-    </row>
-    <row r="15" ht="15.5" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" ht="15.5" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="D14" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s" s="25">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s" s="25">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s" s="26">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" ht="71.75" customHeight="1">
+      <c r="A15" s="19">
+        <v>43849</v>
+      </c>
+      <c r="B15" t="s" s="20">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s" s="25">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s" s="25">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s" s="25">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s" s="26">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" ht="93.05" customHeight="1">
+      <c r="A16" s="19">
+        <v>43851</v>
+      </c>
+      <c r="B16" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s" s="25">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s" s="25">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s" s="25">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s" s="26">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" ht="15.5" customHeight="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" ht="15.5" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" ht="15.5" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" ht="15.5" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" ht="15.5" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="34"/>
     </row>
     <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="34"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="34"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="34"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="34"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="26"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="28"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="34"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="28"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="34"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="34"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="26"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="28"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="34"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="28"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="34"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="28"/>
+      <c r="A45" s="31"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="34"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="26"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="28"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="34"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="34"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="26"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="34"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="28"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="34"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="34"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="28"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="34"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="28"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="28"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="34"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="28"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="34"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="26"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="28"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="34"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="28"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="34"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="26"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="28"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="34"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="28"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="34"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="26"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="28"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="34"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="26"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="28"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="34"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="26"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="28"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="34"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="26"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="28"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="34"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="26"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="28"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="34"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="26"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="28"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="34"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="26"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="28"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="34"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="26"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="28"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="34"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="28"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="34"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="26"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="28"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="34"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="26"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="28"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="26"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="28"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="26"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="28"/>
+      <c r="A71" s="31"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="34"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="26"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="28"/>
+      <c r="A72" s="31"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="34"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="26"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="28"/>
+      <c r="A73" s="31"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+      <c r="G73" s="34"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="26"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="28"/>
+      <c r="A74" s="31"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="34"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="26"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="28"/>
+      <c r="A75" s="31"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="34"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="26"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="28"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="34"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="26"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="28"/>
+      <c r="A77" s="31"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="34"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="26"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="28"/>
+      <c r="A78" s="31"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="34"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="26"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="28"/>
+      <c r="A79" s="31"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="34"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="26"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="28"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32"/>
+      <c r="G80" s="34"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="26"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="28"/>
+      <c r="A81" s="31"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="32"/>
+      <c r="G81" s="34"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="26"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="28"/>
+      <c r="A82" s="31"/>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="32"/>
+      <c r="G82" s="34"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="26"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="28"/>
+      <c r="A83" s="31"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="32"/>
+      <c r="G83" s="34"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="26"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="28"/>
+      <c r="A84" s="31"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="34"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="26"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="28"/>
+      <c r="A85" s="31"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="32"/>
+      <c r="G85" s="34"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="26"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="28"/>
+      <c r="A86" s="31"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="32"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="32"/>
+      <c r="G86" s="34"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="26"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="28"/>
+      <c r="A87" s="31"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="32"/>
+      <c r="G87" s="34"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="26"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="28"/>
+      <c r="A88" s="31"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
+      <c r="G88" s="34"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="26"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="28"/>
+      <c r="A89" s="31"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="32"/>
+      <c r="G89" s="34"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="26"/>
-      <c r="B90" s="27"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="28"/>
+      <c r="A90" s="31"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32"/>
+      <c r="G90" s="34"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="26"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="28"/>
+      <c r="A91" s="31"/>
+      <c r="B91" s="32"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="34"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="26"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="28"/>
+      <c r="A92" s="31"/>
+      <c r="B92" s="32"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="32"/>
+      <c r="F92" s="32"/>
+      <c r="G92" s="34"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="26"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="28"/>
+      <c r="A93" s="31"/>
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="34"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="26"/>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="28"/>
+      <c r="A94" s="31"/>
+      <c r="B94" s="32"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="32"/>
+      <c r="G94" s="34"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="26"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="28"/>
+      <c r="A95" s="31"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="34"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="26"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="28"/>
+      <c r="A96" s="31"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="34"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="26"/>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="28"/>
+      <c r="A97" s="31"/>
+      <c r="B97" s="32"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="34"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="26"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="28"/>
+      <c r="A98" s="31"/>
+      <c r="B98" s="32"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="34"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="26"/>
-      <c r="B99" s="27"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="28"/>
+      <c r="A99" s="31"/>
+      <c r="B99" s="32"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="32"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="32"/>
+      <c r="G99" s="34"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="26"/>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="28"/>
+      <c r="A100" s="31"/>
+      <c r="B100" s="32"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="32"/>
+      <c r="E100" s="32"/>
+      <c r="F100" s="32"/>
+      <c r="G100" s="34"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="26"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="28"/>
+      <c r="A101" s="31"/>
+      <c r="B101" s="32"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="32"/>
+      <c r="G101" s="34"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="26"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="28"/>
+      <c r="A102" s="31"/>
+      <c r="B102" s="32"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="32"/>
+      <c r="G102" s="34"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="26"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="28"/>
+      <c r="A103" s="31"/>
+      <c r="B103" s="32"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="32"/>
+      <c r="G103" s="34"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="26"/>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="28"/>
+      <c r="A104" s="31"/>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="34"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="26"/>
-      <c r="B105" s="27"/>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="28"/>
+      <c r="A105" s="31"/>
+      <c r="B105" s="32"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="32"/>
+      <c r="G105" s="34"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="26"/>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="28"/>
+      <c r="A106" s="31"/>
+      <c r="B106" s="32"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="32"/>
+      <c r="G106" s="34"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="26"/>
-      <c r="B107" s="27"/>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="28"/>
+      <c r="A107" s="31"/>
+      <c r="B107" s="32"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="32"/>
+      <c r="G107" s="34"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="26"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="28"/>
+      <c r="A108" s="31"/>
+      <c r="B108" s="32"/>
+      <c r="C108" s="32"/>
+      <c r="D108" s="32"/>
+      <c r="E108" s="32"/>
+      <c r="F108" s="32"/>
+      <c r="G108" s="34"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="26"/>
-      <c r="B109" s="27"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="28"/>
+      <c r="A109" s="31"/>
+      <c r="B109" s="32"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="32"/>
+      <c r="E109" s="32"/>
+      <c r="F109" s="32"/>
+      <c r="G109" s="34"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="26"/>
-      <c r="B110" s="27"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-      <c r="F110" s="27"/>
-      <c r="G110" s="28"/>
+      <c r="A110" s="31"/>
+      <c r="B110" s="32"/>
+      <c r="C110" s="32"/>
+      <c r="D110" s="32"/>
+      <c r="E110" s="32"/>
+      <c r="F110" s="32"/>
+      <c r="G110" s="34"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="26"/>
-      <c r="B111" s="27"/>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="28"/>
+      <c r="A111" s="31"/>
+      <c r="B111" s="32"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="32"/>
+      <c r="E111" s="32"/>
+      <c r="F111" s="32"/>
+      <c r="G111" s="34"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="26"/>
-      <c r="B112" s="27"/>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="28"/>
+      <c r="A112" s="31"/>
+      <c r="B112" s="32"/>
+      <c r="C112" s="32"/>
+      <c r="D112" s="32"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="32"/>
+      <c r="G112" s="34"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="26"/>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="28"/>
+      <c r="A113" s="31"/>
+      <c r="B113" s="32"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="32"/>
+      <c r="E113" s="32"/>
+      <c r="F113" s="32"/>
+      <c r="G113" s="34"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="26"/>
-      <c r="B114" s="27"/>
-      <c r="C114" s="27"/>
-      <c r="D114" s="27"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
-      <c r="G114" s="28"/>
+      <c r="A114" s="31"/>
+      <c r="B114" s="32"/>
+      <c r="C114" s="32"/>
+      <c r="D114" s="32"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="32"/>
+      <c r="G114" s="34"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="26"/>
-      <c r="B115" s="27"/>
-      <c r="C115" s="27"/>
-      <c r="D115" s="27"/>
-      <c r="E115" s="27"/>
-      <c r="F115" s="27"/>
-      <c r="G115" s="28"/>
+      <c r="A115" s="31"/>
+      <c r="B115" s="32"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="32"/>
+      <c r="E115" s="32"/>
+      <c r="F115" s="32"/>
+      <c r="G115" s="34"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="26"/>
-      <c r="B116" s="27"/>
-      <c r="C116" s="27"/>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-      <c r="F116" s="27"/>
-      <c r="G116" s="28"/>
+      <c r="A116" s="31"/>
+      <c r="B116" s="32"/>
+      <c r="C116" s="32"/>
+      <c r="D116" s="32"/>
+      <c r="E116" s="32"/>
+      <c r="F116" s="32"/>
+      <c r="G116" s="34"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="26"/>
-      <c r="B117" s="27"/>
-      <c r="C117" s="27"/>
-      <c r="D117" s="27"/>
-      <c r="E117" s="27"/>
-      <c r="F117" s="27"/>
-      <c r="G117" s="28"/>
+      <c r="A117" s="31"/>
+      <c r="B117" s="32"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="32"/>
+      <c r="E117" s="32"/>
+      <c r="F117" s="32"/>
+      <c r="G117" s="34"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="26"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="27"/>
-      <c r="E118" s="27"/>
-      <c r="F118" s="27"/>
-      <c r="G118" s="28"/>
+      <c r="A118" s="31"/>
+      <c r="B118" s="32"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="32"/>
+      <c r="E118" s="32"/>
+      <c r="F118" s="32"/>
+      <c r="G118" s="34"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="26"/>
-      <c r="B119" s="27"/>
-      <c r="C119" s="27"/>
-      <c r="D119" s="27"/>
-      <c r="E119" s="27"/>
-      <c r="F119" s="27"/>
-      <c r="G119" s="28"/>
+      <c r="A119" s="31"/>
+      <c r="B119" s="32"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="32"/>
+      <c r="E119" s="32"/>
+      <c r="F119" s="32"/>
+      <c r="G119" s="34"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="26"/>
-      <c r="B120" s="27"/>
-      <c r="C120" s="27"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="28"/>
+      <c r="A120" s="31"/>
+      <c r="B120" s="32"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="32"/>
+      <c r="E120" s="32"/>
+      <c r="F120" s="32"/>
+      <c r="G120" s="34"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="26"/>
-      <c r="B121" s="27"/>
-      <c r="C121" s="27"/>
-      <c r="D121" s="27"/>
-      <c r="E121" s="27"/>
-      <c r="F121" s="27"/>
-      <c r="G121" s="28"/>
+      <c r="A121" s="31"/>
+      <c r="B121" s="32"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="32"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="32"/>
+      <c r="G121" s="34"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="26"/>
-      <c r="B122" s="27"/>
-      <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="27"/>
-      <c r="G122" s="28"/>
+      <c r="A122" s="31"/>
+      <c r="B122" s="32"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="32"/>
+      <c r="E122" s="32"/>
+      <c r="F122" s="32"/>
+      <c r="G122" s="34"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="26"/>
-      <c r="B123" s="27"/>
-      <c r="C123" s="27"/>
-      <c r="D123" s="27"/>
-      <c r="E123" s="27"/>
-      <c r="F123" s="27"/>
-      <c r="G123" s="28"/>
+      <c r="A123" s="31"/>
+      <c r="B123" s="32"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="32"/>
+      <c r="E123" s="32"/>
+      <c r="F123" s="32"/>
+      <c r="G123" s="34"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="26"/>
-      <c r="B124" s="27"/>
-      <c r="C124" s="27"/>
-      <c r="D124" s="27"/>
-      <c r="E124" s="27"/>
-      <c r="F124" s="27"/>
-      <c r="G124" s="28"/>
+      <c r="A124" s="31"/>
+      <c r="B124" s="32"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="32"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="32"/>
+      <c r="G124" s="34"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="32"/>
-      <c r="B125" s="33"/>
-      <c r="C125" s="33"/>
-      <c r="D125" s="33"/>
-      <c r="E125" s="33"/>
-      <c r="F125" s="33"/>
-      <c r="G125" s="34"/>
+      <c r="A125" s="36"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="37"/>
+      <c r="D125" s="37"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="37"/>
+      <c r="G125" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Diary entry for Lecture_3_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -176,6 +176,72 @@
   </si>
   <si>
     <t>Feeling good! Think the answers were right.</t>
+  </si>
+  <si>
+    <t>Looking forward to listen to Alegria! Every week has been a concept which at first we think is simple to work with but turns out there are a lot of features to a basic concept that doesn’t pass our thoughts. I think we covered reading code in the theoretical sense more or less. Let’s see whats next..</t>
+  </si>
+  <si>
+    <t>We understood what mental models are.. starting with basic examples of how doors work and how we think it works. We quickly learnt how to externalize these mental models in terms of reading code. We learnt how to use the template to answer simple questions of jPacman3 features .  We also learnt about UML diagrams and how to generate them. Finally, we had a Skype session with Alumni, it was great to here her perspectives.</t>
+  </si>
+  <si>
+    <t>Writing events down on paper seemed tedious but helped us understand our thought process as this was a group activity and in explaining why we chose to go to a certain function, we understood how differently one thinks.  Also, writing them down made us realize how many functions we open blindly and not realize that we have been there befog because we didn’t have the habit of tracking, Also, visualizing through UML helped us understand how the different classes were related and it was good to see graphic images than plain code. It was also quick to locate in case of smaller projects. Finally, the Skype call made me realize how Women in Tech are evolving and the different work culture in the industry. Also, reading code is very useful.</t>
+  </si>
+  <si>
+    <t>Feeling motivated after listening to the talk!</t>
+  </si>
+  <si>
+    <t>18:00 - 19:00</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>To look for interesting features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We figured that there were not many classes/functions to analyze. </t>
+  </si>
+  <si>
+    <t>Eventhough the project looked fine in the first glance, once we started examining features, we realized a lot of them were inbuilt library functions. The demo provided along with the project has limited functions that we could explore. Shikun noticed these problems first.</t>
+  </si>
+  <si>
+    <t>Have to find a project again! Tiring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We changed our project to JabRef. We analyzed the UML diagrams. We found two seemingly interesting features. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upon changing our project, we noticed it was easier to find functions and features that interest us. We realized the UML diagram was too large to print. </t>
+  </si>
+  <si>
+    <t>Great start!</t>
+  </si>
+  <si>
+    <t>21:00 - 22:00</t>
+  </si>
+  <si>
+    <t>To finish write up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yitian added the screenshots of user interface. Shikun added the details of the table. I added the code snippets. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was smooth as we have settled on the features. Will review the grammar and edit the document for submission tomorrow. </t>
+  </si>
+  <si>
+    <t>A lot of functions that can be ignored! The project didn’t seem so long anymore.</t>
+  </si>
+  <si>
+    <t>Finalize document and UML diagram for submission.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run over the text in the document.Generated UML diagrams for PDF and printed the UML to show in class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We were satisfied with our write up and the end result for the UML. </t>
+  </si>
+  <si>
+    <t>Good!</t>
   </si>
 </sst>
 </file>
@@ -487,7 +553,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -569,11 +635,20 @@
     <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="8" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -587,13 +662,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1691,7 +1760,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1971,50 +2040,120 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" ht="15.5" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" ht="15.5" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" ht="15.5" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="34"/>
-    </row>
-    <row r="20" ht="15.5" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="34"/>
-    </row>
-    <row r="21" ht="15.5" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="34"/>
+    <row r="17" ht="277" customHeight="1">
+      <c r="A17" s="27">
+        <v>43853</v>
+      </c>
+      <c r="B17" t="s" s="28">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s" s="28">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s" s="21">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s" s="21">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="21">
+        <v>54</v>
+      </c>
+      <c r="G17" t="s" s="22">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" ht="113.05" customHeight="1">
+      <c r="A18" s="19">
+        <v>43855</v>
+      </c>
+      <c r="B18" t="s" s="20">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s" s="29">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s" s="21">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s" s="22">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" ht="71" customHeight="1">
+      <c r="A19" s="19">
+        <v>43857</v>
+      </c>
+      <c r="B19" t="s" s="20">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s" s="30">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s" s="21">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s" s="21">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s" s="22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" ht="84.25" customHeight="1">
+      <c r="A20" s="19">
+        <v>43858</v>
+      </c>
+      <c r="B20" t="s" s="20">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s" s="30">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s" s="21">
+        <v>67</v>
+      </c>
+      <c r="F20" t="s" s="21">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s" s="22">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" ht="73.1" customHeight="1">
+      <c r="A21" s="19">
+        <v>43859</v>
+      </c>
+      <c r="B21" t="s" s="20">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s" s="21">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s" s="21">
+        <v>72</v>
+      </c>
+      <c r="G21" t="s" s="22">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" ht="15.5" customHeight="1">
       <c r="A22" s="31"/>
@@ -2023,934 +2162,925 @@
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="34"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="34"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="34"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="34"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="34"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="34"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="34"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="34"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="31"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="34"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="34"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="34"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="34"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="34"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="34"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="34"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="34"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="34"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="34"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="34"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="34"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="34"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="34"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="31"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="34"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="34"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="34"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="31"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="34"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="34"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="34"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="31"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="34"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="31"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="34"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="31"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="34"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="31"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="34"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="31"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="34"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="31"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="34"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="31"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="34"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="36"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="31"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="34"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="36"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="34"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="31"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="34"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="31"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="34"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="31"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="34"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="34"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="31"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="34"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="31"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="34"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="31"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="34"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="31"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="34"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="34"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="31"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="34"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="31"/>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="34"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="31"/>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="34"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="31"/>
-      <c r="B71" s="32"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="34"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="34"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="34"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="31"/>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="34"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="31"/>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="34"/>
+      <c r="A75" s="34"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="31"/>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="34"/>
+      <c r="A76" s="34"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="31"/>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="34"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="31"/>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="34"/>
+      <c r="A78" s="34"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="35"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="31"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="34"/>
+      <c r="A79" s="34"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="35"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="31"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="34"/>
+      <c r="A80" s="34"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="35"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="34"/>
+      <c r="A81" s="34"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="35"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="31"/>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="34"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="34"/>
+      <c r="A83" s="34"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="31"/>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="34"/>
+      <c r="A84" s="34"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="31"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="34"/>
+      <c r="A85" s="34"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
+      <c r="D85" s="35"/>
+      <c r="E85" s="35"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="31"/>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="34"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
+      <c r="E86" s="35"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="31"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="34"/>
+      <c r="A87" s="34"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="35"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="35"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="31"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="34"/>
+      <c r="A88" s="34"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="35"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="31"/>
-      <c r="B89" s="32"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="32"/>
-      <c r="F89" s="32"/>
-      <c r="G89" s="34"/>
+      <c r="A89" s="34"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="35"/>
+      <c r="E89" s="35"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="31"/>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="32"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="32"/>
-      <c r="G90" s="34"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="35"/>
+      <c r="E90" s="35"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="31"/>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="34"/>
+      <c r="A91" s="34"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="35"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="31"/>
-      <c r="B92" s="32"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="34"/>
+      <c r="A92" s="34"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="35"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="31"/>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="34"/>
+      <c r="A93" s="34"/>
+      <c r="B93" s="35"/>
+      <c r="C93" s="35"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="31"/>
-      <c r="B94" s="32"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="34"/>
+      <c r="A94" s="34"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="35"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="31"/>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="34"/>
+      <c r="A95" s="34"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="31"/>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="32"/>
-      <c r="G96" s="34"/>
+      <c r="A96" s="34"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="31"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="34"/>
+      <c r="A97" s="34"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="31"/>
-      <c r="B98" s="32"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="32"/>
-      <c r="E98" s="32"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="34"/>
+      <c r="A98" s="34"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="35"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="31"/>
-      <c r="B99" s="32"/>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="32"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="34"/>
+      <c r="A99" s="34"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="35"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="31"/>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32"/>
-      <c r="D100" s="32"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="34"/>
+      <c r="A100" s="34"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+      <c r="E100" s="35"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="31"/>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="32"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="34"/>
+      <c r="A101" s="34"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="35"/>
+      <c r="F101" s="35"/>
+      <c r="G101" s="36"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="31"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="34"/>
+      <c r="A102" s="34"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
+      <c r="E102" s="35"/>
+      <c r="F102" s="35"/>
+      <c r="G102" s="36"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="31"/>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="32"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="32"/>
-      <c r="G103" s="34"/>
+      <c r="A103" s="34"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="36"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="31"/>
-      <c r="B104" s="32"/>
-      <c r="C104" s="32"/>
-      <c r="D104" s="32"/>
-      <c r="E104" s="32"/>
-      <c r="F104" s="32"/>
-      <c r="G104" s="34"/>
+      <c r="A104" s="34"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
+      <c r="E104" s="35"/>
+      <c r="F104" s="35"/>
+      <c r="G104" s="36"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="31"/>
-      <c r="B105" s="32"/>
-      <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
-      <c r="E105" s="32"/>
-      <c r="F105" s="32"/>
-      <c r="G105" s="34"/>
+      <c r="A105" s="34"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="35"/>
+      <c r="D105" s="35"/>
+      <c r="E105" s="35"/>
+      <c r="F105" s="35"/>
+      <c r="G105" s="36"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="31"/>
-      <c r="B106" s="32"/>
-      <c r="C106" s="32"/>
-      <c r="D106" s="32"/>
-      <c r="E106" s="32"/>
-      <c r="F106" s="32"/>
-      <c r="G106" s="34"/>
+      <c r="A106" s="34"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="35"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="35"/>
+      <c r="G106" s="36"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="31"/>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="34"/>
+      <c r="A107" s="34"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="35"/>
+      <c r="F107" s="35"/>
+      <c r="G107" s="36"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="31"/>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32"/>
-      <c r="D108" s="32"/>
-      <c r="E108" s="32"/>
-      <c r="F108" s="32"/>
-      <c r="G108" s="34"/>
+      <c r="A108" s="34"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="35"/>
+      <c r="E108" s="35"/>
+      <c r="F108" s="35"/>
+      <c r="G108" s="36"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="31"/>
-      <c r="B109" s="32"/>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
-      <c r="E109" s="32"/>
-      <c r="F109" s="32"/>
-      <c r="G109" s="34"/>
+      <c r="A109" s="34"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="35"/>
+      <c r="D109" s="35"/>
+      <c r="E109" s="35"/>
+      <c r="F109" s="35"/>
+      <c r="G109" s="36"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="31"/>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32"/>
-      <c r="D110" s="32"/>
-      <c r="E110" s="32"/>
-      <c r="F110" s="32"/>
-      <c r="G110" s="34"/>
+      <c r="A110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="35"/>
+      <c r="E110" s="35"/>
+      <c r="F110" s="35"/>
+      <c r="G110" s="36"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="31"/>
-      <c r="B111" s="32"/>
-      <c r="C111" s="32"/>
-      <c r="D111" s="32"/>
-      <c r="E111" s="32"/>
-      <c r="F111" s="32"/>
-      <c r="G111" s="34"/>
+      <c r="A111" s="34"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="35"/>
+      <c r="E111" s="35"/>
+      <c r="F111" s="35"/>
+      <c r="G111" s="36"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="31"/>
-      <c r="B112" s="32"/>
-      <c r="C112" s="32"/>
-      <c r="D112" s="32"/>
-      <c r="E112" s="32"/>
-      <c r="F112" s="32"/>
-      <c r="G112" s="34"/>
+      <c r="A112" s="34"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
+      <c r="E112" s="35"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="36"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="31"/>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="32"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="34"/>
+      <c r="A113" s="34"/>
+      <c r="B113" s="35"/>
+      <c r="C113" s="35"/>
+      <c r="D113" s="35"/>
+      <c r="E113" s="35"/>
+      <c r="F113" s="35"/>
+      <c r="G113" s="36"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="31"/>
-      <c r="B114" s="32"/>
-      <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="32"/>
-      <c r="G114" s="34"/>
+      <c r="A114" s="34"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
+      <c r="E114" s="35"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="36"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="31"/>
-      <c r="B115" s="32"/>
-      <c r="C115" s="32"/>
-      <c r="D115" s="32"/>
-      <c r="E115" s="32"/>
-      <c r="F115" s="32"/>
-      <c r="G115" s="34"/>
+      <c r="A115" s="34"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="35"/>
+      <c r="D115" s="35"/>
+      <c r="E115" s="35"/>
+      <c r="F115" s="35"/>
+      <c r="G115" s="36"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="31"/>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32"/>
-      <c r="D116" s="32"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="34"/>
+      <c r="A116" s="34"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="35"/>
+      <c r="D116" s="35"/>
+      <c r="E116" s="35"/>
+      <c r="F116" s="35"/>
+      <c r="G116" s="36"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="31"/>
-      <c r="B117" s="32"/>
-      <c r="C117" s="32"/>
-      <c r="D117" s="32"/>
-      <c r="E117" s="32"/>
-      <c r="F117" s="32"/>
-      <c r="G117" s="34"/>
+      <c r="A117" s="34"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="35"/>
+      <c r="D117" s="35"/>
+      <c r="E117" s="35"/>
+      <c r="F117" s="35"/>
+      <c r="G117" s="36"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="31"/>
-      <c r="B118" s="32"/>
-      <c r="C118" s="32"/>
-      <c r="D118" s="32"/>
-      <c r="E118" s="32"/>
-      <c r="F118" s="32"/>
-      <c r="G118" s="34"/>
+      <c r="A118" s="34"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="35"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="36"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="31"/>
-      <c r="B119" s="32"/>
-      <c r="C119" s="32"/>
-      <c r="D119" s="32"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="32"/>
-      <c r="G119" s="34"/>
+      <c r="A119" s="34"/>
+      <c r="B119" s="35"/>
+      <c r="C119" s="35"/>
+      <c r="D119" s="35"/>
+      <c r="E119" s="35"/>
+      <c r="F119" s="35"/>
+      <c r="G119" s="36"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="31"/>
-      <c r="B120" s="32"/>
-      <c r="C120" s="32"/>
-      <c r="D120" s="32"/>
-      <c r="E120" s="32"/>
-      <c r="F120" s="32"/>
-      <c r="G120" s="34"/>
+      <c r="A120" s="34"/>
+      <c r="B120" s="35"/>
+      <c r="C120" s="35"/>
+      <c r="D120" s="35"/>
+      <c r="E120" s="35"/>
+      <c r="F120" s="35"/>
+      <c r="G120" s="36"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="31"/>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32"/>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="34"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="35"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="35"/>
+      <c r="F121" s="35"/>
+      <c r="G121" s="36"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="31"/>
-      <c r="B122" s="32"/>
-      <c r="C122" s="32"/>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="34"/>
+      <c r="A122" s="34"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="35"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="35"/>
+      <c r="F122" s="35"/>
+      <c r="G122" s="36"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="31"/>
-      <c r="B123" s="32"/>
-      <c r="C123" s="32"/>
-      <c r="D123" s="32"/>
-      <c r="E123" s="32"/>
-      <c r="F123" s="32"/>
-      <c r="G123" s="34"/>
+      <c r="A123" s="34"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="35"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="35"/>
+      <c r="F123" s="35"/>
+      <c r="G123" s="36"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="31"/>
-      <c r="B124" s="32"/>
-      <c r="C124" s="32"/>
-      <c r="D124" s="32"/>
-      <c r="E124" s="32"/>
-      <c r="F124" s="32"/>
-      <c r="G124" s="34"/>
-    </row>
-    <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="36"/>
-      <c r="B125" s="37"/>
-      <c r="C125" s="37"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="38"/>
+      <c r="A124" s="37"/>
+      <c r="B124" s="38"/>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38"/>
+      <c r="E124" s="38"/>
+      <c r="F124" s="38"/>
+      <c r="G124" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Diary entry for Lecture_4_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -242,6 +242,60 @@
   </si>
   <si>
     <t>Good!</t>
+  </si>
+  <si>
+    <t>Looking forward to discuss about our findings as a team and possibly learn the significance of the UML diagrams in detail and the idea behind printing it. Also, wonder who the speaker is gonna be!</t>
+  </si>
+  <si>
+    <t>As expected, we discussed the details and thought process behind choosing the features that we explored. One of the teams bothered to print out the entire UML diagram. We were very confident while answering the questions and also expressed that we did not use the UML diagram much for the project. We learnt about the essence and the professor gave us tips on effective group work. I was very happy to see the Call graphs and sequence diagrams! Finally, we had a talk with Consuelo Lopez who was in various roles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We realized that a lot of teams found the use of UML rather ambiguous. After learning the details of the arrows, I gained some key understanding of the concepts. Since, the professor advised on more face to face meetings and voicing out, we are planning to implement that during out team meeting for next assignment.We also learnt about a situation where the efficiency was reduced by 1000x, was feeling human. It was good to know that experts also make mistakes and we should always explore the choices and not be reserved. Also, taught us the importance of modeling. After viewing the call graphs, I felt that this would be a better use for the assignment. Listening to Consuelo Lopez, reassured me that I will always have the way to explore variety of fields in Software and our purpose is greater than merely coding. </t>
+  </si>
+  <si>
+    <t>Productive! Learnt a lot about visualization. Great to hear the talk.</t>
+  </si>
+  <si>
+    <t>13:30 - 15:00</t>
+  </si>
+  <si>
+    <t>To find two features to build the assignment on!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We figured out the essential features. It was rather easy to identify which are the essential features. </t>
+  </si>
+  <si>
+    <t>Eventhough it was easy to identify the core features as the app has an interactive UI. It was rather difficult to find how we are going to make the package. We settled on the features and identified the key classes using the technique in previous assignment.</t>
+  </si>
+  <si>
+    <t>Feels neutral!</t>
+  </si>
+  <si>
+    <t>To add everything we found to a report and also use the call graphs related to explain further.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished up the write up using several points we found during our discussion and used call graphs to identify some end function and explain the feature. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are satisfied with the write up. I think the Call graphs were more useful than UML diagrams because we couldn’t see many relations or the UML was dense. We abandoned UML altogether. Call graphs were easier to follow and make observations to describe in report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tired. </t>
+  </si>
+  <si>
+    <t>8:00 - 10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run over the report and add any missing code or correct grammar, make sure the packet is understandable and print diagrams. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are satisfied with the report and have done our best to explain with related supporting materials. We printed these call graphs for class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatively easy work as it was just proofreading for today and understanding call graphs. </t>
+  </si>
+  <si>
+    <t>Satisfied!</t>
   </si>
 </sst>
 </file>
@@ -553,7 +607,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -648,13 +702,22 @@
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -2155,50 +2218,106 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-    </row>
-    <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-    </row>
-    <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-    </row>
-    <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
-    </row>
-    <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
+    <row r="22" ht="316.8" customHeight="1">
+      <c r="A22" s="19">
+        <v>43860</v>
+      </c>
+      <c r="B22" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s" s="20">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s" s="20">
+        <v>75</v>
+      </c>
+      <c r="F22" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="G22" t="s" s="24">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" ht="107.15" customHeight="1">
+      <c r="A23" s="19">
+        <v>43865</v>
+      </c>
+      <c r="B23" t="s" s="20">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s" s="20">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s" s="20">
+        <v>80</v>
+      </c>
+      <c r="F23" t="s" s="20">
+        <v>81</v>
+      </c>
+      <c r="G23" t="s" s="24">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" ht="101" customHeight="1">
+      <c r="A24" s="19">
+        <v>43866</v>
+      </c>
+      <c r="B24" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s" s="20">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s" s="20">
+        <v>84</v>
+      </c>
+      <c r="F24" t="s" s="20">
+        <v>85</v>
+      </c>
+      <c r="G24" t="s" s="24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" ht="68.5" customHeight="1">
+      <c r="A25" s="19">
+        <v>43867</v>
+      </c>
+      <c r="B25" t="s" s="20">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s" s="20">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s" s="20">
+        <v>89</v>
+      </c>
+      <c r="F25" t="s" s="20">
+        <v>90</v>
+      </c>
+      <c r="G25" t="s" s="24">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" ht="33.85" customHeight="1">
+      <c r="A26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
       <c r="A27" s="34"/>
@@ -2219,868 +2338,868 @@
       <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="39"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="34"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="34"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="39"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="36"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="36"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="34"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="39"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="39"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="39"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="34"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="36"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="39"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="34"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="36"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="39"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="34"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="34"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="36"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="39"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="36"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="36"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="34"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="36"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="39"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="39"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="34"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="34"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="36"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="39"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="34"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="39"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="34"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="39"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="34"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="39"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="34"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="36"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="39"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="34"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="36"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="39"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="34"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="36"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="39"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="34"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="36"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="39"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="34"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="36"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="39"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="34"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="36"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="39"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="34"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="36"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="34"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="36"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="39"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="34"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="36"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="34"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="34"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="36"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="39"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="34"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="36"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="39"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="34"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="36"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="39"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="34"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="36"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="34"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="36"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="34"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="36"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="39"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="34"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="36"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="39"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="34"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="36"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="39"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="34"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="36"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="34"/>
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="36"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="34"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="36"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="39"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="34"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="35"/>
-      <c r="G76" s="36"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="38"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="39"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="34"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="36"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="39"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="34"/>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="36"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="34"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="36"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="34"/>
-      <c r="B80" s="35"/>
-      <c r="C80" s="35"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="36"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="39"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="34"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="35"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="36"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="39"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="34"/>
-      <c r="B82" s="35"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="36"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="34"/>
-      <c r="B83" s="35"/>
-      <c r="C83" s="35"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="36"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="39"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="34"/>
-      <c r="B84" s="35"/>
-      <c r="C84" s="35"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="35"/>
-      <c r="G84" s="36"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="34"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="35"/>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="36"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="39"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="34"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="36"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="39"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="34"/>
-      <c r="B87" s="35"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="36"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="34"/>
-      <c r="B88" s="35"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="36"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="39"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="34"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="35"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="36"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="38"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="39"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="34"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="35"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="36"/>
+      <c r="A90" s="37"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="34"/>
-      <c r="B91" s="35"/>
-      <c r="C91" s="35"/>
-      <c r="D91" s="35"/>
-      <c r="E91" s="35"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="36"/>
+      <c r="A91" s="37"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="34"/>
-      <c r="B92" s="35"/>
-      <c r="C92" s="35"/>
-      <c r="D92" s="35"/>
-      <c r="E92" s="35"/>
-      <c r="F92" s="35"/>
-      <c r="G92" s="36"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="34"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="35"/>
-      <c r="D93" s="35"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="35"/>
-      <c r="G93" s="36"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="39"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="34"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="35"/>
-      <c r="D94" s="35"/>
-      <c r="E94" s="35"/>
-      <c r="F94" s="35"/>
-      <c r="G94" s="36"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="38"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="39"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="34"/>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
-      <c r="D95" s="35"/>
-      <c r="E95" s="35"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="36"/>
+      <c r="A95" s="37"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="39"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="34"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="35"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35"/>
-      <c r="G96" s="36"/>
+      <c r="A96" s="37"/>
+      <c r="B96" s="38"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="38"/>
+      <c r="E96" s="38"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="39"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="34"/>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="35"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="36"/>
+      <c r="A97" s="37"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="38"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="39"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="34"/>
-      <c r="B98" s="35"/>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="36"/>
+      <c r="A98" s="37"/>
+      <c r="B98" s="38"/>
+      <c r="C98" s="38"/>
+      <c r="D98" s="38"/>
+      <c r="E98" s="38"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="39"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="34"/>
-      <c r="B99" s="35"/>
-      <c r="C99" s="35"/>
-      <c r="D99" s="35"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="36"/>
+      <c r="A99" s="37"/>
+      <c r="B99" s="38"/>
+      <c r="C99" s="38"/>
+      <c r="D99" s="38"/>
+      <c r="E99" s="38"/>
+      <c r="F99" s="38"/>
+      <c r="G99" s="39"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="34"/>
-      <c r="B100" s="35"/>
-      <c r="C100" s="35"/>
-      <c r="D100" s="35"/>
-      <c r="E100" s="35"/>
-      <c r="F100" s="35"/>
-      <c r="G100" s="36"/>
+      <c r="A100" s="37"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="39"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="34"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="35"/>
-      <c r="D101" s="35"/>
-      <c r="E101" s="35"/>
-      <c r="F101" s="35"/>
-      <c r="G101" s="36"/>
+      <c r="A101" s="37"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="38"/>
+      <c r="E101" s="38"/>
+      <c r="F101" s="38"/>
+      <c r="G101" s="39"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="34"/>
-      <c r="B102" s="35"/>
-      <c r="C102" s="35"/>
-      <c r="D102" s="35"/>
-      <c r="E102" s="35"/>
-      <c r="F102" s="35"/>
-      <c r="G102" s="36"/>
+      <c r="A102" s="37"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38"/>
+      <c r="G102" s="39"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="34"/>
-      <c r="B103" s="35"/>
-      <c r="C103" s="35"/>
-      <c r="D103" s="35"/>
-      <c r="E103" s="35"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="36"/>
+      <c r="A103" s="37"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38"/>
+      <c r="E103" s="38"/>
+      <c r="F103" s="38"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="34"/>
-      <c r="B104" s="35"/>
-      <c r="C104" s="35"/>
-      <c r="D104" s="35"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="36"/>
+      <c r="A104" s="37"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="39"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="34"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="35"/>
-      <c r="D105" s="35"/>
-      <c r="E105" s="35"/>
-      <c r="F105" s="35"/>
-      <c r="G105" s="36"/>
+      <c r="A105" s="37"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="34"/>
-      <c r="B106" s="35"/>
-      <c r="C106" s="35"/>
-      <c r="D106" s="35"/>
-      <c r="E106" s="35"/>
-      <c r="F106" s="35"/>
-      <c r="G106" s="36"/>
+      <c r="A106" s="37"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="38"/>
+      <c r="E106" s="38"/>
+      <c r="F106" s="38"/>
+      <c r="G106" s="39"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="34"/>
-      <c r="B107" s="35"/>
-      <c r="C107" s="35"/>
-      <c r="D107" s="35"/>
-      <c r="E107" s="35"/>
-      <c r="F107" s="35"/>
-      <c r="G107" s="36"/>
+      <c r="A107" s="37"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="38"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="39"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="34"/>
-      <c r="B108" s="35"/>
-      <c r="C108" s="35"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="35"/>
-      <c r="F108" s="35"/>
-      <c r="G108" s="36"/>
+      <c r="A108" s="37"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="38"/>
+      <c r="D108" s="38"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="39"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="34"/>
-      <c r="B109" s="35"/>
-      <c r="C109" s="35"/>
-      <c r="D109" s="35"/>
-      <c r="E109" s="35"/>
-      <c r="F109" s="35"/>
-      <c r="G109" s="36"/>
+      <c r="A109" s="37"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="38"/>
+      <c r="D109" s="38"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
+      <c r="G109" s="39"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="34"/>
-      <c r="B110" s="35"/>
-      <c r="C110" s="35"/>
-      <c r="D110" s="35"/>
-      <c r="E110" s="35"/>
-      <c r="F110" s="35"/>
-      <c r="G110" s="36"/>
+      <c r="A110" s="37"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="38"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="34"/>
-      <c r="B111" s="35"/>
-      <c r="C111" s="35"/>
-      <c r="D111" s="35"/>
-      <c r="E111" s="35"/>
-      <c r="F111" s="35"/>
-      <c r="G111" s="36"/>
+      <c r="A111" s="37"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="38"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="34"/>
-      <c r="B112" s="35"/>
-      <c r="C112" s="35"/>
-      <c r="D112" s="35"/>
-      <c r="E112" s="35"/>
-      <c r="F112" s="35"/>
-      <c r="G112" s="36"/>
+      <c r="A112" s="37"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="34"/>
-      <c r="B113" s="35"/>
-      <c r="C113" s="35"/>
-      <c r="D113" s="35"/>
-      <c r="E113" s="35"/>
-      <c r="F113" s="35"/>
-      <c r="G113" s="36"/>
+      <c r="A113" s="37"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="38"/>
+      <c r="E113" s="38"/>
+      <c r="F113" s="38"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="34"/>
-      <c r="B114" s="35"/>
-      <c r="C114" s="35"/>
-      <c r="D114" s="35"/>
-      <c r="E114" s="35"/>
-      <c r="F114" s="35"/>
-      <c r="G114" s="36"/>
+      <c r="A114" s="37"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="39"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="34"/>
-      <c r="B115" s="35"/>
-      <c r="C115" s="35"/>
-      <c r="D115" s="35"/>
-      <c r="E115" s="35"/>
-      <c r="F115" s="35"/>
-      <c r="G115" s="36"/>
+      <c r="A115" s="37"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38"/>
+      <c r="E115" s="38"/>
+      <c r="F115" s="38"/>
+      <c r="G115" s="39"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="34"/>
-      <c r="B116" s="35"/>
-      <c r="C116" s="35"/>
-      <c r="D116" s="35"/>
-      <c r="E116" s="35"/>
-      <c r="F116" s="35"/>
-      <c r="G116" s="36"/>
+      <c r="A116" s="37"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="39"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="34"/>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
-      <c r="D117" s="35"/>
-      <c r="E117" s="35"/>
-      <c r="F117" s="35"/>
-      <c r="G117" s="36"/>
+      <c r="A117" s="37"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="38"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="38"/>
+      <c r="G117" s="39"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="34"/>
-      <c r="B118" s="35"/>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="36"/>
+      <c r="A118" s="37"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38"/>
+      <c r="E118" s="38"/>
+      <c r="F118" s="38"/>
+      <c r="G118" s="39"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="34"/>
-      <c r="B119" s="35"/>
-      <c r="C119" s="35"/>
-      <c r="D119" s="35"/>
-      <c r="E119" s="35"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="36"/>
+      <c r="A119" s="37"/>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38"/>
+      <c r="E119" s="38"/>
+      <c r="F119" s="38"/>
+      <c r="G119" s="39"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="34"/>
-      <c r="B120" s="35"/>
-      <c r="C120" s="35"/>
-      <c r="D120" s="35"/>
-      <c r="E120" s="35"/>
-      <c r="F120" s="35"/>
-      <c r="G120" s="36"/>
+      <c r="A120" s="37"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="38"/>
+      <c r="D120" s="38"/>
+      <c r="E120" s="38"/>
+      <c r="F120" s="38"/>
+      <c r="G120" s="39"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="34"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="35"/>
-      <c r="D121" s="35"/>
-      <c r="E121" s="35"/>
-      <c r="F121" s="35"/>
-      <c r="G121" s="36"/>
+      <c r="A121" s="37"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="38"/>
+      <c r="D121" s="38"/>
+      <c r="E121" s="38"/>
+      <c r="F121" s="38"/>
+      <c r="G121" s="39"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="34"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="35"/>
-      <c r="D122" s="35"/>
-      <c r="E122" s="35"/>
-      <c r="F122" s="35"/>
-      <c r="G122" s="36"/>
+      <c r="A122" s="37"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="38"/>
+      <c r="D122" s="38"/>
+      <c r="E122" s="38"/>
+      <c r="F122" s="38"/>
+      <c r="G122" s="39"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="34"/>
-      <c r="B123" s="35"/>
-      <c r="C123" s="35"/>
-      <c r="D123" s="35"/>
-      <c r="E123" s="35"/>
-      <c r="F123" s="35"/>
-      <c r="G123" s="36"/>
+      <c r="A123" s="37"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="38"/>
+      <c r="E123" s="38"/>
+      <c r="F123" s="38"/>
+      <c r="G123" s="39"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="37"/>
-      <c r="B124" s="38"/>
-      <c r="C124" s="38"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="38"/>
-      <c r="F124" s="38"/>
-      <c r="G124" s="39"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="41"/>
+      <c r="C124" s="41"/>
+      <c r="D124" s="41"/>
+      <c r="E124" s="41"/>
+      <c r="F124" s="41"/>
+      <c r="G124" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Diary entry for Lecture_4_Santhiya_Nagarajan (#270)
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -242,6 +242,60 @@
   </si>
   <si>
     <t>Good!</t>
+  </si>
+  <si>
+    <t>Looking forward to discuss about our findings as a team and possibly learn the significance of the UML diagrams in detail and the idea behind printing it. Also, wonder who the speaker is gonna be!</t>
+  </si>
+  <si>
+    <t>As expected, we discussed the details and thought process behind choosing the features that we explored. One of the teams bothered to print out the entire UML diagram. We were very confident while answering the questions and also expressed that we did not use the UML diagram much for the project. We learnt about the essence and the professor gave us tips on effective group work. I was very happy to see the Call graphs and sequence diagrams! Finally, we had a talk with Consuelo Lopez who was in various roles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We realized that a lot of teams found the use of UML rather ambiguous. After learning the details of the arrows, I gained some key understanding of the concepts. Since, the professor advised on more face to face meetings and voicing out, we are planning to implement that during out team meeting for next assignment.We also learnt about a situation where the efficiency was reduced by 1000x, was feeling human. It was good to know that experts also make mistakes and we should always explore the choices and not be reserved. Also, taught us the importance of modeling. After viewing the call graphs, I felt that this would be a better use for the assignment. Listening to Consuelo Lopez, reassured me that I will always have the way to explore variety of fields in Software and our purpose is greater than merely coding. </t>
+  </si>
+  <si>
+    <t>Productive! Learnt a lot about visualization. Great to hear the talk.</t>
+  </si>
+  <si>
+    <t>13:30 - 15:00</t>
+  </si>
+  <si>
+    <t>To find two features to build the assignment on!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We figured out the essential features. It was rather easy to identify which are the essential features. </t>
+  </si>
+  <si>
+    <t>Eventhough it was easy to identify the core features as the app has an interactive UI. It was rather difficult to find how we are going to make the package. We settled on the features and identified the key classes using the technique in previous assignment.</t>
+  </si>
+  <si>
+    <t>Feels neutral!</t>
+  </si>
+  <si>
+    <t>To add everything we found to a report and also use the call graphs related to explain further.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished up the write up using several points we found during our discussion and used call graphs to identify some end function and explain the feature. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are satisfied with the write up. I think the Call graphs were more useful than UML diagrams because we couldn’t see many relations or the UML was dense. We abandoned UML altogether. Call graphs were easier to follow and make observations to describe in report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tired. </t>
+  </si>
+  <si>
+    <t>8:00 - 10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run over the report and add any missing code or correct grammar, make sure the packet is understandable and print diagrams. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are satisfied with the report and have done our best to explain with related supporting materials. We printed these call graphs for class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatively easy work as it was just proofreading for today and understanding call graphs. </t>
+  </si>
+  <si>
+    <t>Satisfied!</t>
   </si>
 </sst>
 </file>
@@ -553,7 +607,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -648,13 +702,22 @@
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -2155,50 +2218,106 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-    </row>
-    <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-    </row>
-    <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-    </row>
-    <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
-    </row>
-    <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
+    <row r="22" ht="316.8" customHeight="1">
+      <c r="A22" s="19">
+        <v>43860</v>
+      </c>
+      <c r="B22" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s" s="20">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s" s="20">
+        <v>75</v>
+      </c>
+      <c r="F22" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="G22" t="s" s="24">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" ht="107.15" customHeight="1">
+      <c r="A23" s="19">
+        <v>43865</v>
+      </c>
+      <c r="B23" t="s" s="20">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s" s="20">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s" s="20">
+        <v>80</v>
+      </c>
+      <c r="F23" t="s" s="20">
+        <v>81</v>
+      </c>
+      <c r="G23" t="s" s="24">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" ht="101" customHeight="1">
+      <c r="A24" s="19">
+        <v>43866</v>
+      </c>
+      <c r="B24" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s" s="20">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s" s="20">
+        <v>84</v>
+      </c>
+      <c r="F24" t="s" s="20">
+        <v>85</v>
+      </c>
+      <c r="G24" t="s" s="24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" ht="68.5" customHeight="1">
+      <c r="A25" s="19">
+        <v>43867</v>
+      </c>
+      <c r="B25" t="s" s="20">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s" s="20">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s" s="20">
+        <v>89</v>
+      </c>
+      <c r="F25" t="s" s="20">
+        <v>90</v>
+      </c>
+      <c r="G25" t="s" s="24">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" ht="33.85" customHeight="1">
+      <c r="A26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
       <c r="A27" s="34"/>
@@ -2219,868 +2338,868 @@
       <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="39"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="34"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="34"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="39"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="36"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="36"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="34"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="39"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="39"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="39"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="34"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="36"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="39"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="34"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="36"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="39"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="34"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="34"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="36"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="39"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="36"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="36"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="34"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="36"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="39"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="39"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="34"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="34"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="36"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="39"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="34"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="39"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="34"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="39"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="34"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="39"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="34"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="36"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="39"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="34"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="36"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="39"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="34"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="36"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="39"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="34"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="36"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="39"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="34"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="36"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="39"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="34"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="36"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="39"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="34"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="36"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="34"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="36"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="39"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="34"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="36"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="34"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="34"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="36"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="39"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="34"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="36"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="39"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="34"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="36"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="39"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="34"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="36"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="34"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="36"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="34"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="36"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="39"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="34"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="36"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="39"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="34"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="36"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="39"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="34"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="36"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="34"/>
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="36"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="34"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="36"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="39"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="34"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="35"/>
-      <c r="G76" s="36"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="38"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="39"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="34"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="36"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="39"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="34"/>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="36"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="34"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="36"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="34"/>
-      <c r="B80" s="35"/>
-      <c r="C80" s="35"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="36"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="39"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="34"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="35"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="36"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="39"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="34"/>
-      <c r="B82" s="35"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="36"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="34"/>
-      <c r="B83" s="35"/>
-      <c r="C83" s="35"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="36"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="39"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="34"/>
-      <c r="B84" s="35"/>
-      <c r="C84" s="35"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="35"/>
-      <c r="G84" s="36"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="34"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="35"/>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="36"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="39"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="34"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="36"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="39"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="34"/>
-      <c r="B87" s="35"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="36"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="34"/>
-      <c r="B88" s="35"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="36"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="39"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="34"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="35"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="36"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="38"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="39"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="34"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="35"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="36"/>
+      <c r="A90" s="37"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="34"/>
-      <c r="B91" s="35"/>
-      <c r="C91" s="35"/>
-      <c r="D91" s="35"/>
-      <c r="E91" s="35"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="36"/>
+      <c r="A91" s="37"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="34"/>
-      <c r="B92" s="35"/>
-      <c r="C92" s="35"/>
-      <c r="D92" s="35"/>
-      <c r="E92" s="35"/>
-      <c r="F92" s="35"/>
-      <c r="G92" s="36"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="34"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="35"/>
-      <c r="D93" s="35"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="35"/>
-      <c r="G93" s="36"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="39"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="34"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="35"/>
-      <c r="D94" s="35"/>
-      <c r="E94" s="35"/>
-      <c r="F94" s="35"/>
-      <c r="G94" s="36"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="38"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="39"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="34"/>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
-      <c r="D95" s="35"/>
-      <c r="E95" s="35"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="36"/>
+      <c r="A95" s="37"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="39"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="34"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="35"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35"/>
-      <c r="G96" s="36"/>
+      <c r="A96" s="37"/>
+      <c r="B96" s="38"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="38"/>
+      <c r="E96" s="38"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="39"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="34"/>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="35"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="36"/>
+      <c r="A97" s="37"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="38"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="39"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="34"/>
-      <c r="B98" s="35"/>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="36"/>
+      <c r="A98" s="37"/>
+      <c r="B98" s="38"/>
+      <c r="C98" s="38"/>
+      <c r="D98" s="38"/>
+      <c r="E98" s="38"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="39"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="34"/>
-      <c r="B99" s="35"/>
-      <c r="C99" s="35"/>
-      <c r="D99" s="35"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="36"/>
+      <c r="A99" s="37"/>
+      <c r="B99" s="38"/>
+      <c r="C99" s="38"/>
+      <c r="D99" s="38"/>
+      <c r="E99" s="38"/>
+      <c r="F99" s="38"/>
+      <c r="G99" s="39"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="34"/>
-      <c r="B100" s="35"/>
-      <c r="C100" s="35"/>
-      <c r="D100" s="35"/>
-      <c r="E100" s="35"/>
-      <c r="F100" s="35"/>
-      <c r="G100" s="36"/>
+      <c r="A100" s="37"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="39"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="34"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="35"/>
-      <c r="D101" s="35"/>
-      <c r="E101" s="35"/>
-      <c r="F101" s="35"/>
-      <c r="G101" s="36"/>
+      <c r="A101" s="37"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="38"/>
+      <c r="E101" s="38"/>
+      <c r="F101" s="38"/>
+      <c r="G101" s="39"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="34"/>
-      <c r="B102" s="35"/>
-      <c r="C102" s="35"/>
-      <c r="D102" s="35"/>
-      <c r="E102" s="35"/>
-      <c r="F102" s="35"/>
-      <c r="G102" s="36"/>
+      <c r="A102" s="37"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38"/>
+      <c r="G102" s="39"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="34"/>
-      <c r="B103" s="35"/>
-      <c r="C103" s="35"/>
-      <c r="D103" s="35"/>
-      <c r="E103" s="35"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="36"/>
+      <c r="A103" s="37"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38"/>
+      <c r="E103" s="38"/>
+      <c r="F103" s="38"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="34"/>
-      <c r="B104" s="35"/>
-      <c r="C104" s="35"/>
-      <c r="D104" s="35"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="36"/>
+      <c r="A104" s="37"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="39"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="34"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="35"/>
-      <c r="D105" s="35"/>
-      <c r="E105" s="35"/>
-      <c r="F105" s="35"/>
-      <c r="G105" s="36"/>
+      <c r="A105" s="37"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="34"/>
-      <c r="B106" s="35"/>
-      <c r="C106" s="35"/>
-      <c r="D106" s="35"/>
-      <c r="E106" s="35"/>
-      <c r="F106" s="35"/>
-      <c r="G106" s="36"/>
+      <c r="A106" s="37"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="38"/>
+      <c r="E106" s="38"/>
+      <c r="F106" s="38"/>
+      <c r="G106" s="39"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="34"/>
-      <c r="B107" s="35"/>
-      <c r="C107" s="35"/>
-      <c r="D107" s="35"/>
-      <c r="E107" s="35"/>
-      <c r="F107" s="35"/>
-      <c r="G107" s="36"/>
+      <c r="A107" s="37"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="38"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="39"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="34"/>
-      <c r="B108" s="35"/>
-      <c r="C108" s="35"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="35"/>
-      <c r="F108" s="35"/>
-      <c r="G108" s="36"/>
+      <c r="A108" s="37"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="38"/>
+      <c r="D108" s="38"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="39"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="34"/>
-      <c r="B109" s="35"/>
-      <c r="C109" s="35"/>
-      <c r="D109" s="35"/>
-      <c r="E109" s="35"/>
-      <c r="F109" s="35"/>
-      <c r="G109" s="36"/>
+      <c r="A109" s="37"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="38"/>
+      <c r="D109" s="38"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
+      <c r="G109" s="39"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="34"/>
-      <c r="B110" s="35"/>
-      <c r="C110" s="35"/>
-      <c r="D110" s="35"/>
-      <c r="E110" s="35"/>
-      <c r="F110" s="35"/>
-      <c r="G110" s="36"/>
+      <c r="A110" s="37"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="38"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="34"/>
-      <c r="B111" s="35"/>
-      <c r="C111" s="35"/>
-      <c r="D111" s="35"/>
-      <c r="E111" s="35"/>
-      <c r="F111" s="35"/>
-      <c r="G111" s="36"/>
+      <c r="A111" s="37"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="38"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="34"/>
-      <c r="B112" s="35"/>
-      <c r="C112" s="35"/>
-      <c r="D112" s="35"/>
-      <c r="E112" s="35"/>
-      <c r="F112" s="35"/>
-      <c r="G112" s="36"/>
+      <c r="A112" s="37"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="34"/>
-      <c r="B113" s="35"/>
-      <c r="C113" s="35"/>
-      <c r="D113" s="35"/>
-      <c r="E113" s="35"/>
-      <c r="F113" s="35"/>
-      <c r="G113" s="36"/>
+      <c r="A113" s="37"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="38"/>
+      <c r="E113" s="38"/>
+      <c r="F113" s="38"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="34"/>
-      <c r="B114" s="35"/>
-      <c r="C114" s="35"/>
-      <c r="D114" s="35"/>
-      <c r="E114" s="35"/>
-      <c r="F114" s="35"/>
-      <c r="G114" s="36"/>
+      <c r="A114" s="37"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="39"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="34"/>
-      <c r="B115" s="35"/>
-      <c r="C115" s="35"/>
-      <c r="D115" s="35"/>
-      <c r="E115" s="35"/>
-      <c r="F115" s="35"/>
-      <c r="G115" s="36"/>
+      <c r="A115" s="37"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38"/>
+      <c r="E115" s="38"/>
+      <c r="F115" s="38"/>
+      <c r="G115" s="39"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="34"/>
-      <c r="B116" s="35"/>
-      <c r="C116" s="35"/>
-      <c r="D116" s="35"/>
-      <c r="E116" s="35"/>
-      <c r="F116" s="35"/>
-      <c r="G116" s="36"/>
+      <c r="A116" s="37"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="39"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="34"/>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
-      <c r="D117" s="35"/>
-      <c r="E117" s="35"/>
-      <c r="F117" s="35"/>
-      <c r="G117" s="36"/>
+      <c r="A117" s="37"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="38"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="38"/>
+      <c r="G117" s="39"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="34"/>
-      <c r="B118" s="35"/>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="36"/>
+      <c r="A118" s="37"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38"/>
+      <c r="E118" s="38"/>
+      <c r="F118" s="38"/>
+      <c r="G118" s="39"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="34"/>
-      <c r="B119" s="35"/>
-      <c r="C119" s="35"/>
-      <c r="D119" s="35"/>
-      <c r="E119" s="35"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="36"/>
+      <c r="A119" s="37"/>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38"/>
+      <c r="E119" s="38"/>
+      <c r="F119" s="38"/>
+      <c r="G119" s="39"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="34"/>
-      <c r="B120" s="35"/>
-      <c r="C120" s="35"/>
-      <c r="D120" s="35"/>
-      <c r="E120" s="35"/>
-      <c r="F120" s="35"/>
-      <c r="G120" s="36"/>
+      <c r="A120" s="37"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="38"/>
+      <c r="D120" s="38"/>
+      <c r="E120" s="38"/>
+      <c r="F120" s="38"/>
+      <c r="G120" s="39"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="34"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="35"/>
-      <c r="D121" s="35"/>
-      <c r="E121" s="35"/>
-      <c r="F121" s="35"/>
-      <c r="G121" s="36"/>
+      <c r="A121" s="37"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="38"/>
+      <c r="D121" s="38"/>
+      <c r="E121" s="38"/>
+      <c r="F121" s="38"/>
+      <c r="G121" s="39"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="34"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="35"/>
-      <c r="D122" s="35"/>
-      <c r="E122" s="35"/>
-      <c r="F122" s="35"/>
-      <c r="G122" s="36"/>
+      <c r="A122" s="37"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="38"/>
+      <c r="D122" s="38"/>
+      <c r="E122" s="38"/>
+      <c r="F122" s="38"/>
+      <c r="G122" s="39"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="34"/>
-      <c r="B123" s="35"/>
-      <c r="C123" s="35"/>
-      <c r="D123" s="35"/>
-      <c r="E123" s="35"/>
-      <c r="F123" s="35"/>
-      <c r="G123" s="36"/>
+      <c r="A123" s="37"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="38"/>
+      <c r="E123" s="38"/>
+      <c r="F123" s="38"/>
+      <c r="G123" s="39"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="37"/>
-      <c r="B124" s="38"/>
-      <c r="C124" s="38"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="38"/>
-      <c r="F124" s="38"/>
-      <c r="G124" s="39"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="41"/>
+      <c r="C124" s="41"/>
+      <c r="D124" s="41"/>
+      <c r="E124" s="41"/>
+      <c r="F124" s="41"/>
+      <c r="G124" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Diary entry for Lecture_5_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -296,6 +296,60 @@
   </si>
   <si>
     <t>Satisfied!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking forward to discuss the assignment. This one was rather vague and was hard to convince each other and explain what has to go in the packet. Anyway, expecting questions regarding assignments and also looking forward to the speaker. </t>
+  </si>
+  <si>
+    <t>Learnt other KEP. The professor questioned me about hello word and I merged to get it right. Had an explanation from Rafael for the byte parsing, I couldn’t understand. It was nice that the professor appreciated this acceptance later. Finally we went back to our favorite JPacman and performed a few exercieses. We had a talk from Christopher in Consultant Alliance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I realized that it is very important to be skeptical about the code. Always be out for catching mistakes. Also, understood the importance of asking questions and even if you are smart, there might be problems in communicating your mental model to others, which is externalising. Therefor, it is a skill that has to honed further and will help during whiteboard interviews, etc. When we were doing the Paceman exercise, I realized it is normal to take a long time to figure some details out and we should not shy away from it and give our best shot at it. Finally, listening to the speaker who has had a lot of experience in the field. I realized the importance of clean code, documentation and optimization. I’m glad he has such a great passion and it was obvious in the way he was speaking. Also, something to take away from the class today. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tensed about the exam. Hope the practical goes fine as I have problems with importing projects at times. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on Lecture 1,2 </t>
+  </si>
+  <si>
+    <t>Finished working on Lecture 1</t>
+  </si>
+  <si>
+    <t>Feel how deep we have gone with the topic, where in lecture 1 it merely started with reading code, interesting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleepy! Hope to finish the rest tomorrow. </t>
+  </si>
+  <si>
+    <t>10:00 - 14:00</t>
+  </si>
+  <si>
+    <t>Meet Kaj to discuss about assignment, Work on remaining lectures</t>
+  </si>
+  <si>
+    <t>Got insights about our assignment and where we could improve or future, Finished working on remaining lectures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventhough we were pretty confident about our approach, we realized that our documentation was not up to mark. That is in externalizing our thought process to a third person to the project. We have promised to work harder for future as a team and to provide concise and descriptive documentation with relation to the existing diagrams. Also, finished on lectures. Lecture 5 seems to be dense with the content.  </t>
+  </si>
+  <si>
+    <t>Tired.</t>
+  </si>
+  <si>
+    <t>9:00 - 11:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revise notes written, practice basic plugins </t>
+  </si>
+  <si>
+    <t>Finished revising for the exam</t>
+  </si>
+  <si>
+    <t>Thought it was only five lectures, but the content is pretty dense. Hope to remember the concepts and have the time to think about answers</t>
+  </si>
+  <si>
+    <t>Feeling tensed about the exam! But have prepared enough. Hope it goes well.</t>
   </si>
 </sst>
 </file>
@@ -607,7 +661,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -633,37 +687,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
@@ -671,35 +725,23 @@
     <xf numFmtId="49" fontId="11" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="59" fontId="8" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
@@ -719,23 +761,14 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1952,16 +1985,16 @@
       <c r="C10" t="s" s="20">
         <v>15</v>
       </c>
-      <c r="D10" t="s" s="21">
+      <c r="D10" t="s" s="20">
         <v>16</v>
       </c>
-      <c r="E10" t="s" s="21">
+      <c r="E10" t="s" s="20">
         <v>17</v>
       </c>
-      <c r="F10" t="s" s="21">
+      <c r="F10" t="s" s="20">
         <v>18</v>
       </c>
-      <c r="G10" t="s" s="22">
+      <c r="G10" t="s" s="21">
         <v>19</v>
       </c>
     </row>
@@ -1975,16 +2008,16 @@
       <c r="C11" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="D11" t="s" s="21">
+      <c r="D11" t="s" s="20">
         <v>22</v>
       </c>
-      <c r="E11" t="s" s="21">
+      <c r="E11" t="s" s="20">
         <v>23</v>
       </c>
-      <c r="F11" t="s" s="21">
+      <c r="F11" t="s" s="20">
         <v>24</v>
       </c>
-      <c r="G11" t="s" s="22">
+      <c r="G11" t="s" s="21">
         <v>25</v>
       </c>
     </row>
@@ -1998,21 +2031,21 @@
       <c r="C12" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="D12" t="s" s="21">
+      <c r="D12" t="s" s="20">
         <v>27</v>
       </c>
-      <c r="E12" t="s" s="21">
+      <c r="E12" t="s" s="20">
         <v>28</v>
       </c>
-      <c r="F12" t="s" s="21">
+      <c r="F12" t="s" s="20">
         <v>29</v>
       </c>
-      <c r="G12" t="s" s="22">
+      <c r="G12" t="s" s="21">
         <v>30</v>
       </c>
     </row>
     <row r="13" ht="129" customHeight="1">
-      <c r="A13" t="s" s="23">
+      <c r="A13" t="s" s="22">
         <v>31</v>
       </c>
       <c r="B13" t="s" s="20">
@@ -2021,16 +2054,16 @@
       <c r="C13" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="D13" t="s" s="21">
+      <c r="D13" t="s" s="20">
         <v>32</v>
       </c>
-      <c r="E13" t="s" s="21">
+      <c r="E13" t="s" s="20">
         <v>33</v>
       </c>
-      <c r="F13" t="s" s="21">
+      <c r="F13" t="s" s="20">
         <v>34</v>
       </c>
-      <c r="G13" t="s" s="24">
+      <c r="G13" t="s" s="21">
         <v>35</v>
       </c>
     </row>
@@ -2044,16 +2077,16 @@
       <c r="C14" t="s" s="20">
         <v>37</v>
       </c>
-      <c r="D14" t="s" s="25">
+      <c r="D14" t="s" s="20">
         <v>38</v>
       </c>
-      <c r="E14" t="s" s="25">
+      <c r="E14" t="s" s="20">
         <v>39</v>
       </c>
-      <c r="F14" t="s" s="25">
+      <c r="F14" t="s" s="20">
         <v>40</v>
       </c>
-      <c r="G14" t="s" s="26">
+      <c r="G14" t="s" s="21">
         <v>41</v>
       </c>
     </row>
@@ -2067,16 +2100,16 @@
       <c r="C15" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="D15" t="s" s="25">
+      <c r="D15" t="s" s="20">
         <v>43</v>
       </c>
-      <c r="E15" t="s" s="25">
+      <c r="E15" t="s" s="20">
         <v>44</v>
       </c>
-      <c r="F15" t="s" s="25">
+      <c r="F15" t="s" s="20">
         <v>45</v>
       </c>
-      <c r="G15" t="s" s="26">
+      <c r="G15" t="s" s="21">
         <v>46</v>
       </c>
     </row>
@@ -2090,39 +2123,39 @@
       <c r="C16" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="D16" t="s" s="25">
+      <c r="D16" t="s" s="20">
         <v>48</v>
       </c>
-      <c r="E16" t="s" s="25">
+      <c r="E16" t="s" s="20">
         <v>49</v>
       </c>
-      <c r="F16" t="s" s="25">
+      <c r="F16" t="s" s="20">
         <v>50</v>
       </c>
-      <c r="G16" t="s" s="26">
+      <c r="G16" t="s" s="21">
         <v>51</v>
       </c>
     </row>
     <row r="17" ht="277" customHeight="1">
-      <c r="A17" s="27">
+      <c r="A17" s="23">
         <v>43853</v>
       </c>
-      <c r="B17" t="s" s="28">
+      <c r="B17" t="s" s="24">
         <v>14</v>
       </c>
-      <c r="C17" t="s" s="28">
+      <c r="C17" t="s" s="24">
         <v>21</v>
       </c>
-      <c r="D17" t="s" s="21">
+      <c r="D17" t="s" s="20">
         <v>52</v>
       </c>
-      <c r="E17" t="s" s="21">
+      <c r="E17" t="s" s="20">
         <v>53</v>
       </c>
-      <c r="F17" t="s" s="21">
+      <c r="F17" t="s" s="20">
         <v>54</v>
       </c>
-      <c r="G17" t="s" s="22">
+      <c r="G17" t="s" s="21">
         <v>55</v>
       </c>
     </row>
@@ -2136,16 +2169,16 @@
       <c r="C18" t="s" s="20">
         <v>57</v>
       </c>
-      <c r="D18" t="s" s="29">
+      <c r="D18" t="s" s="24">
         <v>58</v>
       </c>
-      <c r="E18" t="s" s="21">
+      <c r="E18" t="s" s="20">
         <v>59</v>
       </c>
-      <c r="F18" t="s" s="21">
+      <c r="F18" t="s" s="20">
         <v>60</v>
       </c>
-      <c r="G18" t="s" s="22">
+      <c r="G18" t="s" s="21">
         <v>61</v>
       </c>
     </row>
@@ -2159,16 +2192,16 @@
       <c r="C19" t="s" s="20">
         <v>57</v>
       </c>
-      <c r="D19" t="s" s="30">
+      <c r="D19" t="s" s="25">
         <v>58</v>
       </c>
-      <c r="E19" t="s" s="21">
+      <c r="E19" t="s" s="20">
         <v>62</v>
       </c>
-      <c r="F19" t="s" s="21">
+      <c r="F19" t="s" s="20">
         <v>63</v>
       </c>
-      <c r="G19" t="s" s="22">
+      <c r="G19" t="s" s="21">
         <v>64</v>
       </c>
     </row>
@@ -2182,16 +2215,16 @@
       <c r="C20" t="s" s="20">
         <v>57</v>
       </c>
-      <c r="D20" t="s" s="30">
+      <c r="D20" t="s" s="25">
         <v>66</v>
       </c>
-      <c r="E20" t="s" s="21">
+      <c r="E20" t="s" s="20">
         <v>67</v>
       </c>
-      <c r="F20" t="s" s="21">
+      <c r="F20" t="s" s="20">
         <v>68</v>
       </c>
-      <c r="G20" t="s" s="22">
+      <c r="G20" t="s" s="21">
         <v>69</v>
       </c>
     </row>
@@ -2205,16 +2238,16 @@
       <c r="C21" t="s" s="20">
         <v>57</v>
       </c>
-      <c r="D21" t="s" s="21">
+      <c r="D21" t="s" s="20">
         <v>70</v>
       </c>
-      <c r="E21" t="s" s="21">
+      <c r="E21" t="s" s="20">
         <v>71</v>
       </c>
-      <c r="F21" t="s" s="21">
+      <c r="F21" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="G21" t="s" s="22">
+      <c r="G21" t="s" s="21">
         <v>73</v>
       </c>
     </row>
@@ -2237,7 +2270,7 @@
       <c r="F22" t="s" s="20">
         <v>76</v>
       </c>
-      <c r="G22" t="s" s="24">
+      <c r="G22" t="s" s="21">
         <v>77</v>
       </c>
     </row>
@@ -2260,7 +2293,7 @@
       <c r="F23" t="s" s="20">
         <v>81</v>
       </c>
-      <c r="G23" t="s" s="24">
+      <c r="G23" t="s" s="21">
         <v>82</v>
       </c>
     </row>
@@ -2283,7 +2316,7 @@
       <c r="F24" t="s" s="20">
         <v>85</v>
       </c>
-      <c r="G24" t="s" s="24">
+      <c r="G24" t="s" s="21">
         <v>86</v>
       </c>
     </row>
@@ -2306,900 +2339,956 @@
       <c r="F25" t="s" s="20">
         <v>90</v>
       </c>
-      <c r="G25" t="s" s="24">
+      <c r="G25" t="s" s="21">
         <v>91</v>
       </c>
     </row>
-    <row r="26" ht="33.85" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
-    </row>
-    <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
-    </row>
-    <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="37"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="39"/>
+    <row r="26" ht="304.35" customHeight="1">
+      <c r="A26" s="19">
+        <v>43867</v>
+      </c>
+      <c r="B26" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s" s="20">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s" s="20">
+        <v>93</v>
+      </c>
+      <c r="F26" t="s" s="20">
+        <v>94</v>
+      </c>
+      <c r="G26" t="s" s="21">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" ht="51.45" customHeight="1">
+      <c r="A27" s="19">
+        <v>43872</v>
+      </c>
+      <c r="B27" t="s" s="20">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s" s="20">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s" s="20">
+        <v>97</v>
+      </c>
+      <c r="F27" t="s" s="20">
+        <v>98</v>
+      </c>
+      <c r="G27" t="s" s="21">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" ht="157" customHeight="1">
+      <c r="A28" s="19">
+        <v>43873</v>
+      </c>
+      <c r="B28" t="s" s="20">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s" s="20">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s" s="20">
+        <v>102</v>
+      </c>
+      <c r="F28" t="s" s="20">
+        <v>103</v>
+      </c>
+      <c r="G28" t="s" s="21">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" ht="72.5" customHeight="1">
+      <c r="A29" s="19">
+        <v>43874</v>
+      </c>
+      <c r="B29" t="s" s="20">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s" s="20">
+        <v>106</v>
+      </c>
+      <c r="E29" t="s" s="20">
+        <v>107</v>
+      </c>
+      <c r="F29" t="s" s="20">
+        <v>108</v>
+      </c>
+      <c r="G29" t="s" s="26">
+        <v>109</v>
+      </c>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="39"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="37"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="39"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="37"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="37"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="37"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="39"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="37"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="37"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="37"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="39"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="37"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="37"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="39"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="37"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="39"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="39"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="32"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="37"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="39"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="37"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="39"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="37"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="39"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="37"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="37"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="32"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="37"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="39"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="32"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="37"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="39"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="32"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="37"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="32"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="37"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="39"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="37"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="39"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="32"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="37"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="39"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="37"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="39"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="32"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="37"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="39"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="37"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="39"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="32"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="37"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="39"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="32"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="37"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="39"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="32"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="37"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="39"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="32"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="37"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="39"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="32"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="37"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="39"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="32"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="37"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="39"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="32"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="37"/>
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="32"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="37"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="39"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="32"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="37"/>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="39"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="32"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="37"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="39"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="32"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="37"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="39"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="32"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="37"/>
-      <c r="B69" s="38"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="32"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="37"/>
-      <c r="B70" s="38"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="38"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="39"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="32"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="37"/>
-      <c r="B71" s="38"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="38"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="39"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="32"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="37"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="39"/>
+      <c r="A72" s="30"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="32"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="37"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="39"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="32"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="37"/>
-      <c r="B74" s="38"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="38"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="39"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="32"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="37"/>
-      <c r="B75" s="38"/>
-      <c r="C75" s="38"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="38"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="39"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="32"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="37"/>
-      <c r="B76" s="38"/>
-      <c r="C76" s="38"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="38"/>
-      <c r="F76" s="38"/>
-      <c r="G76" s="39"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="31"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="32"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="37"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="39"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="31"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="32"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="37"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="38"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="39"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="32"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="37"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="38"/>
-      <c r="F79" s="38"/>
-      <c r="G79" s="39"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="32"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="37"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="39"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="37"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="39"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="31"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="32"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="37"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="39"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="32"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="37"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="38"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="39"/>
+      <c r="A83" s="30"/>
+      <c r="B83" s="31"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="31"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="32"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="37"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="38"/>
-      <c r="F84" s="38"/>
-      <c r="G84" s="39"/>
+      <c r="A84" s="30"/>
+      <c r="B84" s="31"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="32"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="37"/>
-      <c r="B85" s="38"/>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="39"/>
+      <c r="A85" s="30"/>
+      <c r="B85" s="31"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="32"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="37"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="39"/>
+      <c r="A86" s="30"/>
+      <c r="B86" s="31"/>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="32"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="37"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="39"/>
+      <c r="A87" s="30"/>
+      <c r="B87" s="31"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="32"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="37"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="38"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="39"/>
+      <c r="A88" s="30"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="31"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="32"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="37"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="38"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="38"/>
-      <c r="G89" s="39"/>
+      <c r="A89" s="30"/>
+      <c r="B89" s="31"/>
+      <c r="C89" s="31"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="31"/>
+      <c r="F89" s="31"/>
+      <c r="G89" s="32"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="37"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="39"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="31"/>
+      <c r="C90" s="31"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="31"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="32"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="37"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="39"/>
+      <c r="A91" s="30"/>
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="32"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="37"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="39"/>
+      <c r="A92" s="30"/>
+      <c r="B92" s="31"/>
+      <c r="C92" s="31"/>
+      <c r="D92" s="31"/>
+      <c r="E92" s="31"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="32"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="37"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="38"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="38"/>
-      <c r="F93" s="38"/>
-      <c r="G93" s="39"/>
+      <c r="A93" s="30"/>
+      <c r="B93" s="31"/>
+      <c r="C93" s="31"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="31"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="32"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="37"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="38"/>
-      <c r="F94" s="38"/>
-      <c r="G94" s="39"/>
+      <c r="A94" s="30"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="31"/>
+      <c r="D94" s="31"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="32"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="37"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="38"/>
-      <c r="F95" s="38"/>
-      <c r="G95" s="39"/>
+      <c r="A95" s="30"/>
+      <c r="B95" s="31"/>
+      <c r="C95" s="31"/>
+      <c r="D95" s="31"/>
+      <c r="E95" s="31"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="32"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="37"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="38"/>
-      <c r="F96" s="38"/>
-      <c r="G96" s="39"/>
+      <c r="A96" s="30"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="31"/>
+      <c r="D96" s="31"/>
+      <c r="E96" s="31"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="32"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="37"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="38"/>
-      <c r="F97" s="38"/>
-      <c r="G97" s="39"/>
+      <c r="A97" s="30"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="31"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="31"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="32"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="37"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="38"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="38"/>
-      <c r="F98" s="38"/>
-      <c r="G98" s="39"/>
+      <c r="A98" s="30"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="31"/>
+      <c r="D98" s="31"/>
+      <c r="E98" s="31"/>
+      <c r="F98" s="31"/>
+      <c r="G98" s="32"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="37"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="38"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="38"/>
-      <c r="F99" s="38"/>
-      <c r="G99" s="39"/>
+      <c r="A99" s="30"/>
+      <c r="B99" s="31"/>
+      <c r="C99" s="31"/>
+      <c r="D99" s="31"/>
+      <c r="E99" s="31"/>
+      <c r="F99" s="31"/>
+      <c r="G99" s="32"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="37"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="38"/>
-      <c r="D100" s="38"/>
-      <c r="E100" s="38"/>
-      <c r="F100" s="38"/>
-      <c r="G100" s="39"/>
+      <c r="A100" s="30"/>
+      <c r="B100" s="31"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="31"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="32"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="37"/>
-      <c r="B101" s="38"/>
-      <c r="C101" s="38"/>
-      <c r="D101" s="38"/>
-      <c r="E101" s="38"/>
-      <c r="F101" s="38"/>
-      <c r="G101" s="39"/>
+      <c r="A101" s="30"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="31"/>
+      <c r="E101" s="31"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="32"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="37"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="38"/>
-      <c r="F102" s="38"/>
-      <c r="G102" s="39"/>
+      <c r="A102" s="30"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="31"/>
+      <c r="D102" s="31"/>
+      <c r="E102" s="31"/>
+      <c r="F102" s="31"/>
+      <c r="G102" s="32"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="37"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="38"/>
-      <c r="F103" s="38"/>
-      <c r="G103" s="39"/>
+      <c r="A103" s="30"/>
+      <c r="B103" s="31"/>
+      <c r="C103" s="31"/>
+      <c r="D103" s="31"/>
+      <c r="E103" s="31"/>
+      <c r="F103" s="31"/>
+      <c r="G103" s="32"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="37"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="38"/>
-      <c r="F104" s="38"/>
-      <c r="G104" s="39"/>
+      <c r="A104" s="30"/>
+      <c r="B104" s="31"/>
+      <c r="C104" s="31"/>
+      <c r="D104" s="31"/>
+      <c r="E104" s="31"/>
+      <c r="F104" s="31"/>
+      <c r="G104" s="32"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="37"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="38"/>
-      <c r="D105" s="38"/>
-      <c r="E105" s="38"/>
-      <c r="F105" s="38"/>
-      <c r="G105" s="39"/>
+      <c r="A105" s="30"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="31"/>
+      <c r="D105" s="31"/>
+      <c r="E105" s="31"/>
+      <c r="F105" s="31"/>
+      <c r="G105" s="32"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="37"/>
-      <c r="B106" s="38"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="38"/>
-      <c r="E106" s="38"/>
-      <c r="F106" s="38"/>
-      <c r="G106" s="39"/>
+      <c r="A106" s="30"/>
+      <c r="B106" s="31"/>
+      <c r="C106" s="31"/>
+      <c r="D106" s="31"/>
+      <c r="E106" s="31"/>
+      <c r="F106" s="31"/>
+      <c r="G106" s="32"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="37"/>
-      <c r="B107" s="38"/>
-      <c r="C107" s="38"/>
-      <c r="D107" s="38"/>
-      <c r="E107" s="38"/>
-      <c r="F107" s="38"/>
-      <c r="G107" s="39"/>
+      <c r="A107" s="30"/>
+      <c r="B107" s="31"/>
+      <c r="C107" s="31"/>
+      <c r="D107" s="31"/>
+      <c r="E107" s="31"/>
+      <c r="F107" s="31"/>
+      <c r="G107" s="32"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="37"/>
-      <c r="B108" s="38"/>
-      <c r="C108" s="38"/>
-      <c r="D108" s="38"/>
-      <c r="E108" s="38"/>
-      <c r="F108" s="38"/>
-      <c r="G108" s="39"/>
+      <c r="A108" s="30"/>
+      <c r="B108" s="31"/>
+      <c r="C108" s="31"/>
+      <c r="D108" s="31"/>
+      <c r="E108" s="31"/>
+      <c r="F108" s="31"/>
+      <c r="G108" s="32"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="37"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="38"/>
-      <c r="D109" s="38"/>
-      <c r="E109" s="38"/>
-      <c r="F109" s="38"/>
-      <c r="G109" s="39"/>
+      <c r="A109" s="30"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="31"/>
+      <c r="D109" s="31"/>
+      <c r="E109" s="31"/>
+      <c r="F109" s="31"/>
+      <c r="G109" s="32"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="37"/>
-      <c r="B110" s="38"/>
-      <c r="C110" s="38"/>
-      <c r="D110" s="38"/>
-      <c r="E110" s="38"/>
-      <c r="F110" s="38"/>
-      <c r="G110" s="39"/>
+      <c r="A110" s="30"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="31"/>
+      <c r="D110" s="31"/>
+      <c r="E110" s="31"/>
+      <c r="F110" s="31"/>
+      <c r="G110" s="32"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="37"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="38"/>
-      <c r="D111" s="38"/>
-      <c r="E111" s="38"/>
-      <c r="F111" s="38"/>
-      <c r="G111" s="39"/>
+      <c r="A111" s="30"/>
+      <c r="B111" s="31"/>
+      <c r="C111" s="31"/>
+      <c r="D111" s="31"/>
+      <c r="E111" s="31"/>
+      <c r="F111" s="31"/>
+      <c r="G111" s="32"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="37"/>
-      <c r="B112" s="38"/>
-      <c r="C112" s="38"/>
-      <c r="D112" s="38"/>
-      <c r="E112" s="38"/>
-      <c r="F112" s="38"/>
-      <c r="G112" s="39"/>
+      <c r="A112" s="30"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="31"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="31"/>
+      <c r="F112" s="31"/>
+      <c r="G112" s="32"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="37"/>
-      <c r="B113" s="38"/>
-      <c r="C113" s="38"/>
-      <c r="D113" s="38"/>
-      <c r="E113" s="38"/>
-      <c r="F113" s="38"/>
-      <c r="G113" s="39"/>
+      <c r="A113" s="30"/>
+      <c r="B113" s="31"/>
+      <c r="C113" s="31"/>
+      <c r="D113" s="31"/>
+      <c r="E113" s="31"/>
+      <c r="F113" s="31"/>
+      <c r="G113" s="32"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="37"/>
-      <c r="B114" s="38"/>
-      <c r="C114" s="38"/>
-      <c r="D114" s="38"/>
-      <c r="E114" s="38"/>
-      <c r="F114" s="38"/>
-      <c r="G114" s="39"/>
+      <c r="A114" s="30"/>
+      <c r="B114" s="31"/>
+      <c r="C114" s="31"/>
+      <c r="D114" s="31"/>
+      <c r="E114" s="31"/>
+      <c r="F114" s="31"/>
+      <c r="G114" s="32"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="37"/>
-      <c r="B115" s="38"/>
-      <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
-      <c r="E115" s="38"/>
-      <c r="F115" s="38"/>
-      <c r="G115" s="39"/>
+      <c r="A115" s="30"/>
+      <c r="B115" s="31"/>
+      <c r="C115" s="31"/>
+      <c r="D115" s="31"/>
+      <c r="E115" s="31"/>
+      <c r="F115" s="31"/>
+      <c r="G115" s="32"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="37"/>
-      <c r="B116" s="38"/>
-      <c r="C116" s="38"/>
-      <c r="D116" s="38"/>
-      <c r="E116" s="38"/>
-      <c r="F116" s="38"/>
-      <c r="G116" s="39"/>
+      <c r="A116" s="30"/>
+      <c r="B116" s="31"/>
+      <c r="C116" s="31"/>
+      <c r="D116" s="31"/>
+      <c r="E116" s="31"/>
+      <c r="F116" s="31"/>
+      <c r="G116" s="32"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="37"/>
-      <c r="B117" s="38"/>
-      <c r="C117" s="38"/>
-      <c r="D117" s="38"/>
-      <c r="E117" s="38"/>
-      <c r="F117" s="38"/>
-      <c r="G117" s="39"/>
+      <c r="A117" s="30"/>
+      <c r="B117" s="31"/>
+      <c r="C117" s="31"/>
+      <c r="D117" s="31"/>
+      <c r="E117" s="31"/>
+      <c r="F117" s="31"/>
+      <c r="G117" s="32"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="37"/>
-      <c r="B118" s="38"/>
-      <c r="C118" s="38"/>
-      <c r="D118" s="38"/>
-      <c r="E118" s="38"/>
-      <c r="F118" s="38"/>
-      <c r="G118" s="39"/>
+      <c r="A118" s="30"/>
+      <c r="B118" s="31"/>
+      <c r="C118" s="31"/>
+      <c r="D118" s="31"/>
+      <c r="E118" s="31"/>
+      <c r="F118" s="31"/>
+      <c r="G118" s="32"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="37"/>
-      <c r="B119" s="38"/>
-      <c r="C119" s="38"/>
-      <c r="D119" s="38"/>
-      <c r="E119" s="38"/>
-      <c r="F119" s="38"/>
-      <c r="G119" s="39"/>
+      <c r="A119" s="30"/>
+      <c r="B119" s="31"/>
+      <c r="C119" s="31"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="31"/>
+      <c r="F119" s="31"/>
+      <c r="G119" s="32"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="37"/>
-      <c r="B120" s="38"/>
-      <c r="C120" s="38"/>
-      <c r="D120" s="38"/>
-      <c r="E120" s="38"/>
-      <c r="F120" s="38"/>
-      <c r="G120" s="39"/>
+      <c r="A120" s="30"/>
+      <c r="B120" s="31"/>
+      <c r="C120" s="31"/>
+      <c r="D120" s="31"/>
+      <c r="E120" s="31"/>
+      <c r="F120" s="31"/>
+      <c r="G120" s="32"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="37"/>
-      <c r="B121" s="38"/>
-      <c r="C121" s="38"/>
-      <c r="D121" s="38"/>
-      <c r="E121" s="38"/>
-      <c r="F121" s="38"/>
-      <c r="G121" s="39"/>
+      <c r="A121" s="30"/>
+      <c r="B121" s="31"/>
+      <c r="C121" s="31"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="31"/>
+      <c r="F121" s="31"/>
+      <c r="G121" s="32"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="37"/>
-      <c r="B122" s="38"/>
-      <c r="C122" s="38"/>
-      <c r="D122" s="38"/>
-      <c r="E122" s="38"/>
-      <c r="F122" s="38"/>
-      <c r="G122" s="39"/>
+      <c r="A122" s="30"/>
+      <c r="B122" s="31"/>
+      <c r="C122" s="31"/>
+      <c r="D122" s="31"/>
+      <c r="E122" s="31"/>
+      <c r="F122" s="31"/>
+      <c r="G122" s="32"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="37"/>
-      <c r="B123" s="38"/>
-      <c r="C123" s="38"/>
-      <c r="D123" s="38"/>
-      <c r="E123" s="38"/>
-      <c r="F123" s="38"/>
-      <c r="G123" s="39"/>
+      <c r="A123" s="30"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="31"/>
+      <c r="D123" s="31"/>
+      <c r="E123" s="31"/>
+      <c r="F123" s="31"/>
+      <c r="G123" s="32"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="40"/>
-      <c r="B124" s="41"/>
-      <c r="C124" s="41"/>
-      <c r="D124" s="41"/>
-      <c r="E124" s="41"/>
-      <c r="F124" s="41"/>
-      <c r="G124" s="42"/>
+      <c r="A124" s="33"/>
+      <c r="B124" s="34"/>
+      <c r="C124" s="34"/>
+      <c r="D124" s="34"/>
+      <c r="E124" s="34"/>
+      <c r="F124" s="34"/>
+      <c r="G124" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Diary entry for Lecture_6_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -350,6 +350,60 @@
   </si>
   <si>
     <t>Feeling tensed about the exam! But have prepared enough. Hope it goes well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish exam on time, hope to remember what I learned. Hope we have the energy to concentrate on the lecture. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished exam on time, remembered most of the details. Successfully sat through the lecture. The concepts were explained well and were easy to comprehend.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felt like the time was just right, didn’t have time to go through the paper, should work at a faster pace for the finals. Handwriting got shabby towards the end, hopefully Kaj understands. The practical part of the exam was rather confusing to settle on. I think I spent a lot of time and couldn’t really write a satisfying answer. We discussed the survey results. Glad to know that a lot of people felt the same. Finally, we had a lecture about Stakeholders, developers and the bigger picture of the system. Really liked the KEP#9, because I tend to go for a run every time I am stressed and it has worked wonders. </t>
+  </si>
+  <si>
+    <t>16:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Discuss the functionalities of various features and developers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We found a lot of features related to the functionalities and had to categorize it. We also managed to find the key developers in JabRef’s GitHub. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After finding the functionalities, it was rather hard for each of us to agree whether it was functional or non-functional. For example, integration to environment, Built in custom export formats, etc. After agreeing on that, it was also hard for us to decide which four to put up for each. They all seemed equally crucial. </t>
+  </si>
+  <si>
+    <t>Fruitful Discussion</t>
+  </si>
+  <si>
+    <t>21:00 -23:00</t>
+  </si>
+  <si>
+    <t>Final discussion about functionalities, find stakeholder information, find what’s unique about the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We managed to find information about stakeholders after a tedious search of going among the donations, finding survey information related to JabRef. We were able to find unique features by reading reviews on JabRef </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After going through the survey details, we were somewhat able to settle on stakeholders. With a wide possible range of users mainly academics, we were able to find two universities that primarily used JabRef. We were happy that we could find this crucial info on time. After much thought, we finished the write up for features. While reading the reviews, we were leaning more towards what other people found useful about the system as well. This gave us a better sense of choosing the unique feature among our own contradicting beliefs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy that we could find related info which is very useful to write up the report. </t>
+  </si>
+  <si>
+    <t>7:30 - 9:00</t>
+  </si>
+  <si>
+    <t>Add references to the report</t>
+  </si>
+  <si>
+    <t>Finished adding references to the report, made changes with grammar and was focussing on building a concise report.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glad that we finished the report. Hopefully scores well. We have also included the references to ease the search for info for the grader. </t>
   </si>
 </sst>
 </file>
@@ -2435,50 +2489,106 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-    </row>
-    <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="32"/>
+    <row r="30" ht="227" customHeight="1">
+      <c r="A30" s="19">
+        <v>43874</v>
+      </c>
+      <c r="B30" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s" s="20">
+        <v>110</v>
+      </c>
+      <c r="E30" t="s" s="20">
+        <v>111</v>
+      </c>
+      <c r="F30" t="s" s="20">
+        <v>112</v>
+      </c>
+      <c r="G30" t="s" s="21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" ht="136.85" customHeight="1">
+      <c r="A31" s="19">
+        <v>43878</v>
+      </c>
+      <c r="B31" t="s" s="20">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s" s="20">
+        <v>115</v>
+      </c>
+      <c r="E31" t="s" s="20">
+        <v>116</v>
+      </c>
+      <c r="F31" t="s" s="20">
+        <v>117</v>
+      </c>
+      <c r="G31" t="s" s="21">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" ht="214.5" customHeight="1">
+      <c r="A32" s="19">
+        <v>43880</v>
+      </c>
+      <c r="B32" t="s" s="20">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s" s="20">
+        <v>120</v>
+      </c>
+      <c r="E32" t="s" s="20">
+        <v>121</v>
+      </c>
+      <c r="F32" t="s" s="20">
+        <v>122</v>
+      </c>
+      <c r="G32" t="s" s="21">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" ht="72.2" customHeight="1">
+      <c r="A33" s="19">
+        <v>43881</v>
+      </c>
+      <c r="B33" t="s" s="20">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s" s="20">
+        <v>125</v>
+      </c>
+      <c r="E33" t="s" s="20">
+        <v>126</v>
+      </c>
+      <c r="F33" t="s" s="20">
+        <v>127</v>
+      </c>
+      <c r="G33" t="s" s="21">
+        <v>91</v>
+      </c>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="32"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
       <c r="A35" s="30"/>

</xml_diff>

<commit_message>
Added Diary entry for Lecture_7_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -404,6 +404,66 @@
   </si>
   <si>
     <t xml:space="preserve">Glad that we finished the report. Hopefully scores well. We have also included the references to ease the search for info for the grader. </t>
+  </si>
+  <si>
+    <t>Looking forward to discuss the assignment as we had hard time settling on the essential functional and non-functional features, want to hear other groups’ opinions. Let’s see if we get our midterms today, kind of nervous. Also, looking forward to the speaker!</t>
+  </si>
+  <si>
+    <t>We discussed on the features we found interesting, it was nice to hear the different security concerns or portability features from others’ systems. We studied few more key concepts. Followed by crash coursing Software Architecture. We motivated the architecture behind jPacman 3 with partners. We also learnt about the social context and the different standards that one should adhere to while making a pull request. Finally, had an interesting conversation with Sara and Omar!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When questioned about the suppliers, nobody that was questioned was able to answer the details which was sad since we spent the previous week working for the assignment. While looking for the architectural pattern behind jPacman, I understood the various ways of thinking, bottom up or higher level abstractions.  Even though, we all knew roughly about the general principles, doing the exercise made as not so confident about our understanding of MVC and the arrows that connect these sectors. It was easier to understand once we grouped different sections in UML. Finally, it was interesting to listen to Sara and Omar. Sara seemed nervous in the newer settings which again reassures that even if we are experts in our field, it is normal to feel human, to be tensed when addressing a crowd, etc. Personally, my favorite till date, as she was very genuine with her answers and also because she changed majors as well and seems to be doing what she is passionate about. </t>
+  </si>
+  <si>
+    <t>Tired with the overflow of info in the later part but the drawings for KEP are very interesting and well done!</t>
+  </si>
+  <si>
+    <t>Discuss architecture, run over the assignment 2 resubmission</t>
+  </si>
+  <si>
+    <t>We managed to look at the folder structures and settle on a MVC like pattern for as-implemented. As-intended architecture, we looked at closed pull requests/issues and were able to see the core developers take on it. Finished rewriting the Assignment 2 and submitted</t>
+  </si>
+  <si>
+    <t>We noticed a lot of interdependencies among different components of the core structures in the software. This violates a true MVC design. We were happy to roughly come up with the architectural design after the fruitful discussion</t>
+  </si>
+  <si>
+    <t>Challenging discussion</t>
+  </si>
+  <si>
+    <t>Finish deciding on interesting pull requests and issues</t>
+  </si>
+  <si>
+    <t>We managed to settle on five interesting pull requests and issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While reading through the various pull requests and issues, it was funny how the conversations are among the developers and the submitters. We also understand how not to write commit messages or how bland certain statements are. Also the feedback from the developers helps us in understanding the thought process they go through. We noticed a checklist for the submission which was interesting and the first time I had seen such a thing on GitHub.  </t>
+  </si>
+  <si>
+    <t>Interesting!</t>
+  </si>
+  <si>
+    <t>Finish write up on Social Context</t>
+  </si>
+  <si>
+    <t>We managed to find resources that can aid us with developing the social context of the system</t>
+  </si>
+  <si>
+    <t>We looked up the pulse in GitHub page and we were also surprised at how active the developers are, like merging within two days! Glad that we chose an active project and hopefully we can contribute effectively</t>
+  </si>
+  <si>
+    <t>8:00 - 12:00</t>
+  </si>
+  <si>
+    <t>Finish the entire write up, combine the individual parts we organized</t>
+  </si>
+  <si>
+    <t>We managed to finish the write up, didn’t really think it would take this long as we had already discussed the key essence and architectural patterns</t>
+  </si>
+  <si>
+    <t>There were a lot of confusion with regards to adhering to the architectural because we had interdependencies in a pure MVC. Hope we addressed these carefully in the report for Kajo to understand.  Social context section was a lot of work and effort. Nevertheless, we feel more confident about making a pull request and know where to go find the details. Feels like we know the project very well conceptually and somewhat working wise.</t>
+  </si>
+  <si>
+    <t>Praise the documentation and blog of JabRef.</t>
   </si>
 </sst>
 </file>
@@ -2581,59 +2641,129 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29"/>
-    </row>
-    <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="32"/>
-    </row>
-    <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="32"/>
-    </row>
-    <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="30"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
-    </row>
-    <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
+    <row r="34" ht="376.7" customHeight="1">
+      <c r="A34" s="19">
+        <v>43881</v>
+      </c>
+      <c r="B34" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s" s="20">
+        <v>128</v>
+      </c>
+      <c r="E34" t="s" s="20">
+        <v>129</v>
+      </c>
+      <c r="F34" t="s" s="20">
+        <v>130</v>
+      </c>
+      <c r="G34" t="s" s="21">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" ht="122.45" customHeight="1">
+      <c r="A35" s="19">
+        <v>43883</v>
+      </c>
+      <c r="B35" t="s" s="20">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s" s="20">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s" s="20">
+        <v>133</v>
+      </c>
+      <c r="F35" t="s" s="20">
+        <v>134</v>
+      </c>
+      <c r="G35" t="s" s="21">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" ht="188.55" customHeight="1">
+      <c r="A36" s="19">
+        <v>43886</v>
+      </c>
+      <c r="B36" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s" s="20">
+        <v>136</v>
+      </c>
+      <c r="E36" t="s" s="20">
+        <v>137</v>
+      </c>
+      <c r="F36" t="s" s="20">
+        <v>138</v>
+      </c>
+      <c r="G36" t="s" s="21">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" ht="116.7" customHeight="1">
+      <c r="A37" s="19">
+        <v>43887</v>
+      </c>
+      <c r="B37" t="s" s="20">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D37" t="s" s="20">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s" s="20">
+        <v>141</v>
+      </c>
+      <c r="F37" t="s" s="20">
+        <v>142</v>
+      </c>
+      <c r="G37" t="s" s="21">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" ht="182.7" customHeight="1">
+      <c r="A38" s="19">
+        <v>43888</v>
+      </c>
+      <c r="B38" t="s" s="20">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s" s="20">
+        <v>144</v>
+      </c>
+      <c r="E38" t="s" s="20">
+        <v>145</v>
+      </c>
+      <c r="F38" t="s" s="20">
+        <v>146</v>
+      </c>
+      <c r="G38" t="s" s="21">
+        <v>147</v>
+      </c>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="32"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
       <c r="A40" s="30"/>

</xml_diff>

<commit_message>
Added Diary entry for Lecture_7_Santhiya_Nagarajan (#413)
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -404,6 +404,66 @@
   </si>
   <si>
     <t xml:space="preserve">Glad that we finished the report. Hopefully scores well. We have also included the references to ease the search for info for the grader. </t>
+  </si>
+  <si>
+    <t>Looking forward to discuss the assignment as we had hard time settling on the essential functional and non-functional features, want to hear other groups’ opinions. Let’s see if we get our midterms today, kind of nervous. Also, looking forward to the speaker!</t>
+  </si>
+  <si>
+    <t>We discussed on the features we found interesting, it was nice to hear the different security concerns or portability features from others’ systems. We studied few more key concepts. Followed by crash coursing Software Architecture. We motivated the architecture behind jPacman 3 with partners. We also learnt about the social context and the different standards that one should adhere to while making a pull request. Finally, had an interesting conversation with Sara and Omar!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When questioned about the suppliers, nobody that was questioned was able to answer the details which was sad since we spent the previous week working for the assignment. While looking for the architectural pattern behind jPacman, I understood the various ways of thinking, bottom up or higher level abstractions.  Even though, we all knew roughly about the general principles, doing the exercise made as not so confident about our understanding of MVC and the arrows that connect these sectors. It was easier to understand once we grouped different sections in UML. Finally, it was interesting to listen to Sara and Omar. Sara seemed nervous in the newer settings which again reassures that even if we are experts in our field, it is normal to feel human, to be tensed when addressing a crowd, etc. Personally, my favorite till date, as she was very genuine with her answers and also because she changed majors as well and seems to be doing what she is passionate about. </t>
+  </si>
+  <si>
+    <t>Tired with the overflow of info in the later part but the drawings for KEP are very interesting and well done!</t>
+  </si>
+  <si>
+    <t>Discuss architecture, run over the assignment 2 resubmission</t>
+  </si>
+  <si>
+    <t>We managed to look at the folder structures and settle on a MVC like pattern for as-implemented. As-intended architecture, we looked at closed pull requests/issues and were able to see the core developers take on it. Finished rewriting the Assignment 2 and submitted</t>
+  </si>
+  <si>
+    <t>We noticed a lot of interdependencies among different components of the core structures in the software. This violates a true MVC design. We were happy to roughly come up with the architectural design after the fruitful discussion</t>
+  </si>
+  <si>
+    <t>Challenging discussion</t>
+  </si>
+  <si>
+    <t>Finish deciding on interesting pull requests and issues</t>
+  </si>
+  <si>
+    <t>We managed to settle on five interesting pull requests and issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While reading through the various pull requests and issues, it was funny how the conversations are among the developers and the submitters. We also understand how not to write commit messages or how bland certain statements are. Also the feedback from the developers helps us in understanding the thought process they go through. We noticed a checklist for the submission which was interesting and the first time I had seen such a thing on GitHub.  </t>
+  </si>
+  <si>
+    <t>Interesting!</t>
+  </si>
+  <si>
+    <t>Finish write up on Social Context</t>
+  </si>
+  <si>
+    <t>We managed to find resources that can aid us with developing the social context of the system</t>
+  </si>
+  <si>
+    <t>We looked up the pulse in GitHub page and we were also surprised at how active the developers are, like merging within two days! Glad that we chose an active project and hopefully we can contribute effectively</t>
+  </si>
+  <si>
+    <t>8:00 - 12:00</t>
+  </si>
+  <si>
+    <t>Finish the entire write up, combine the individual parts we organized</t>
+  </si>
+  <si>
+    <t>We managed to finish the write up, didn’t really think it would take this long as we had already discussed the key essence and architectural patterns</t>
+  </si>
+  <si>
+    <t>There were a lot of confusion with regards to adhering to the architectural because we had interdependencies in a pure MVC. Hope we addressed these carefully in the report for Kajo to understand.  Social context section was a lot of work and effort. Nevertheless, we feel more confident about making a pull request and know where to go find the details. Feels like we know the project very well conceptually and somewhat working wise.</t>
+  </si>
+  <si>
+    <t>Praise the documentation and blog of JabRef.</t>
   </si>
 </sst>
 </file>
@@ -2581,59 +2641,129 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29"/>
-    </row>
-    <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="32"/>
-    </row>
-    <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="32"/>
-    </row>
-    <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="30"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
-    </row>
-    <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
+    <row r="34" ht="376.7" customHeight="1">
+      <c r="A34" s="19">
+        <v>43881</v>
+      </c>
+      <c r="B34" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s" s="20">
+        <v>128</v>
+      </c>
+      <c r="E34" t="s" s="20">
+        <v>129</v>
+      </c>
+      <c r="F34" t="s" s="20">
+        <v>130</v>
+      </c>
+      <c r="G34" t="s" s="21">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" ht="122.45" customHeight="1">
+      <c r="A35" s="19">
+        <v>43883</v>
+      </c>
+      <c r="B35" t="s" s="20">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s" s="20">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s" s="20">
+        <v>133</v>
+      </c>
+      <c r="F35" t="s" s="20">
+        <v>134</v>
+      </c>
+      <c r="G35" t="s" s="21">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" ht="188.55" customHeight="1">
+      <c r="A36" s="19">
+        <v>43886</v>
+      </c>
+      <c r="B36" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s" s="20">
+        <v>136</v>
+      </c>
+      <c r="E36" t="s" s="20">
+        <v>137</v>
+      </c>
+      <c r="F36" t="s" s="20">
+        <v>138</v>
+      </c>
+      <c r="G36" t="s" s="21">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" ht="116.7" customHeight="1">
+      <c r="A37" s="19">
+        <v>43887</v>
+      </c>
+      <c r="B37" t="s" s="20">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D37" t="s" s="20">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s" s="20">
+        <v>141</v>
+      </c>
+      <c r="F37" t="s" s="20">
+        <v>142</v>
+      </c>
+      <c r="G37" t="s" s="21">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" ht="182.7" customHeight="1">
+      <c r="A38" s="19">
+        <v>43888</v>
+      </c>
+      <c r="B38" t="s" s="20">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s" s="20">
+        <v>144</v>
+      </c>
+      <c r="E38" t="s" s="20">
+        <v>145</v>
+      </c>
+      <c r="F38" t="s" s="20">
+        <v>146</v>
+      </c>
+      <c r="G38" t="s" s="21">
+        <v>147</v>
+      </c>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="32"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
       <c r="A40" s="30"/>

</xml_diff>

<commit_message>
Added Diary entry for Lecture_8_Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -464,6 +464,60 @@
   </si>
   <si>
     <t>Praise the documentation and blog of JabRef.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking forward to discuss our assignment on contribution standards and probably how to make the pull request. Don’t know what is going to be covered this lecture! Looking forward to the guest as usual. </t>
+  </si>
+  <si>
+    <t>We discussed about the architecture and it was great to know that everyone had problems in finding the architecture or settling on a pure style. We faced a lot of difficulties in settling on the report. We learnt more about KEP. The one on invest and save time later is great.Especially because we are all changing majors I guess it is important to understand the root of all the courses than to rush. We learnt about software design patterns and the ducks example helped us in understanding the underlying concept. We had an amazing talk by Alberto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial explanation about DBH and conference helped in understanding design pattern. We were not able to do the practical part so I am guessing the homework will be harder. Finally, listening to Alberto about Astrophysics was great because I could related more as I have done research in Computational Chemistry before with Simulation software that used Fortran. It was great to listen to some Physics again! He is very passionate about his work and it is great to know the various fields that we can work in or contribute to. </t>
+  </si>
+  <si>
+    <t>Feeling tired!</t>
+  </si>
+  <si>
+    <t>18:00-20:00</t>
+  </si>
+  <si>
+    <t>Finalize the issue to solve, Identity two patterns</t>
+  </si>
+  <si>
+    <t>Yitian suggested we address the issue about the titles as it is relatively new and that it was tagged as good for first time contributors. We agreed on this issue after skimming through the others. We came up with basic strategy of the problem and we plan to implement this modification for the pull request. Upon looking for design patterns, we managed to look for keywords like adapter, builder, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I realized that contributing to a project is not that bad after all and we don’t have to know each and every part because we looked into the issue and it said exactly what the problem was. We used the knowledge from previous classes to look for beacons and infant managed to find the algorithm that caused this error and to our surprise this was a concise file. </t>
+  </si>
+  <si>
+    <t>Feeling smart!</t>
+  </si>
+  <si>
+    <t>Submit pull request, Identify three patterns</t>
+  </si>
+  <si>
+    <t>We agreed on the pull request submission and made it as per standards we had found in the previous assignment. We found enum iterator pattern, and it was relatively harder to find the other prototype and factory method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are satisfied that we were able to contribute to the open source community and sure that there will be more comments on the issue. Hope to hear back them in a day as this is a highly active project. While submitting this request, we also came up with a solution for the next week’s assignment. The design patterns were interesting to read and analyse. </t>
+  </si>
+  <si>
+    <t>Feeling motivated to keep track of JabRef and identify minor issues to contribute!</t>
+  </si>
+  <si>
+    <t>21:00-23:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Settle on the design patterns report</t>
+  </si>
+  <si>
+    <t>We finished writing the complete report for the assignment. While we checked the pull request, the developer has indeed got back to us quick. Looking forward to fix the addressed comments</t>
+  </si>
+  <si>
+    <t>We were asked to write test cases for the change we suggested. We are happy that we got a response back and are confident that we can integrate our knowledge from Testing course to write beautiful cases covering the improvement. I liked how detailed the developer had replied, it is easy to understand what he is looking for.</t>
+  </si>
+  <si>
+    <t>Feeling good!</t>
   </si>
 </sst>
 </file>
@@ -2756,50 +2810,106 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="29"/>
-    </row>
-    <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="30"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="32"/>
-    </row>
-    <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
+    <row r="39" ht="199" customHeight="1">
+      <c r="A39" s="19">
+        <v>43888</v>
+      </c>
+      <c r="B39" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s" s="20">
+        <v>148</v>
+      </c>
+      <c r="E39" t="s" s="20">
+        <v>149</v>
+      </c>
+      <c r="F39" t="s" s="20">
+        <v>150</v>
+      </c>
+      <c r="G39" t="s" s="21">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" ht="157" customHeight="1">
+      <c r="A40" s="19">
+        <v>43891</v>
+      </c>
+      <c r="B40" t="s" s="20">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D40" t="s" s="20">
+        <v>153</v>
+      </c>
+      <c r="E40" t="s" s="20">
+        <v>154</v>
+      </c>
+      <c r="F40" t="s" s="20">
+        <v>155</v>
+      </c>
+      <c r="G40" t="s" s="21">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" ht="151.2" customHeight="1">
+      <c r="A41" s="19">
+        <v>43892</v>
+      </c>
+      <c r="B41" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s" s="20">
+        <v>157</v>
+      </c>
+      <c r="E41" t="s" s="20">
+        <v>158</v>
+      </c>
+      <c r="F41" t="s" s="20">
+        <v>159</v>
+      </c>
+      <c r="G41" t="s" s="21">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" ht="129" customHeight="1">
+      <c r="A42" s="19">
+        <v>43894</v>
+      </c>
+      <c r="B42" t="s" s="20">
+        <v>161</v>
+      </c>
+      <c r="C42" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D42" t="s" s="20">
+        <v>162</v>
+      </c>
+      <c r="E42" t="s" s="20">
+        <v>163</v>
+      </c>
+      <c r="F42" t="s" s="20">
+        <v>164</v>
+      </c>
+      <c r="G42" t="s" s="21">
+        <v>165</v>
+      </c>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="30"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="32"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
       <c r="A44" s="30"/>

</xml_diff>